<commit_message>
borrado de Controller2, ciclo de celdas combinadas en Controller
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -7267,6 +7267,23 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="G1:M1"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="T3:V3"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="T13:V13"/>
+    <mergeCell ref="AA33:AC33"/>
+    <mergeCell ref="AA34:AC34"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="L23:N23"/>
+    <mergeCell ref="T23:V23"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="L32:N32"/>
+    <mergeCell ref="T32:V32"/>
+  </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -7833,6 +7850,15 @@
       <c r="H62" s="364"/>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B58:H62"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="J6:P6"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+  </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -8409,6 +8435,15 @@
       <c r="H62" s="393"/>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B58:H62"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="J6:P6"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+  </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -8975,6 +9010,15 @@
       <c r="H62" s="422"/>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B58:H62"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="J6:P6"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+  </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -9551,6 +9595,15 @@
       <c r="H62" s="451"/>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B58:H62"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="J6:P6"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+  </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -10142,6 +10195,15 @@
       <c r="H62" s="124"/>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B58:H62"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="J6:P6"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+  </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -10710,6 +10772,15 @@
       <c r="H61" s="155"/>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B57:H61"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="J6:P6"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+  </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -11306,6 +11377,15 @@
       <c r="H62" s="186"/>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B58:H62"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="J6:P6"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+  </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -11891,6 +11971,15 @@
       <c r="H62" s="217"/>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B58:H62"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="J6:P6"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+  </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -12482,6 +12571,15 @@
       <c r="H62" s="248"/>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B58:H62"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="J6:P6"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+  </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -13052,6 +13150,15 @@
       <c r="H62" s="277"/>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B58:H62"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="J6:P6"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+  </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -13628,6 +13735,15 @@
       <c r="H62" s="306"/>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B58:H62"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="J6:P6"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+  </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -14204,6 +14320,15 @@
       <c r="H62" s="335"/>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B58:H62"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="J6:P6"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+  </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added enterprises new logos and new libraries
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="84">
   <si>
     <t>2021 Calendar</t>
   </si>
@@ -7960,33 +7960,36 @@
       <c r="G15" s="353"/>
     </row>
     <row r="16" ht="14.4" customHeight="true">
-      <c r="B16" s="29" t="n">
+      <c r="B16" s="354" t="n">
         <v>1.0</v>
       </c>
-      <c r="C16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="G16" s="29" t="s">
-        <v>83</v>
+      <c r="C16" s="355"/>
+      <c r="E16" s="355"/>
+      <c r="G16" s="353" t="n">
+        <f>((E16-C16)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="17" ht="14.4" customHeight="true">
-      <c r="B17" s="30" t="n">
+      <c r="B17" s="354" t="n">
         <v>2.0</v>
       </c>
-      <c r="C17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="G17" s="30" t="s">
-        <v>83</v>
+      <c r="C17" s="355"/>
+      <c r="E17" s="355"/>
+      <c r="G17" s="353" t="n">
+        <f>((E17-C17)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="18" ht="14.4" customHeight="true">
-      <c r="B18" s="30" t="n">
+      <c r="B18" s="354" t="n">
         <v>3.0</v>
       </c>
-      <c r="C18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="G18" s="30" t="s">
-        <v>83</v>
+      <c r="C18" s="355"/>
+      <c r="E18" s="355"/>
+      <c r="G18" s="353" t="n">
+        <f>((E18-C18)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="19" ht="14.4" customHeight="true">
@@ -8010,53 +8013,58 @@
       </c>
     </row>
     <row r="21" ht="14.4" customHeight="true">
-      <c r="B21" s="36" t="n">
+      <c r="B21" s="354" t="n">
         <v>6.0</v>
       </c>
-      <c r="C21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="G21" s="36" t="s">
-        <v>83</v>
+      <c r="C21" s="355"/>
+      <c r="E21" s="355"/>
+      <c r="G21" s="353" t="n">
+        <f>((E21-C21)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="22" ht="14.4" customHeight="true">
-      <c r="B22" s="36" t="n">
+      <c r="B22" s="354" t="n">
         <v>7.0</v>
       </c>
-      <c r="C22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="G22" s="36" t="s">
-        <v>83</v>
+      <c r="C22" s="355"/>
+      <c r="E22" s="355"/>
+      <c r="G22" s="353" t="n">
+        <f>((E22-C22)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="23" ht="14.4" customHeight="true">
-      <c r="B23" s="36" t="n">
+      <c r="B23" s="354" t="n">
         <v>8.0</v>
       </c>
-      <c r="C23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="G23" s="36" t="s">
-        <v>83</v>
+      <c r="C23" s="355"/>
+      <c r="E23" s="355"/>
+      <c r="G23" s="353" t="n">
+        <f>((E23-C23)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="24" ht="14.4" customHeight="true">
-      <c r="B24" s="36" t="n">
+      <c r="B24" s="354" t="n">
         <v>9.0</v>
       </c>
-      <c r="C24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="G24" s="36" t="s">
-        <v>83</v>
+      <c r="C24" s="355"/>
+      <c r="E24" s="355"/>
+      <c r="G24" s="353" t="n">
+        <f>((E24-C24)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="25" ht="14.4" customHeight="true">
-      <c r="B25" s="36" t="n">
+      <c r="B25" s="354" t="n">
         <v>10.0</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="G25" s="36" t="s">
-        <v>83</v>
+      <c r="C25" s="355"/>
+      <c r="E25" s="355"/>
+      <c r="G25" s="353" t="n">
+        <f>((E25-C25)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="26" ht="14.4" customHeight="true">
@@ -8080,53 +8088,58 @@
       </c>
     </row>
     <row r="28" ht="14.4" customHeight="true">
-      <c r="B28" s="43" t="n">
+      <c r="B28" s="354" t="n">
         <v>13.0</v>
       </c>
-      <c r="C28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="G28" s="43" t="s">
-        <v>83</v>
+      <c r="C28" s="355"/>
+      <c r="E28" s="355"/>
+      <c r="G28" s="353" t="n">
+        <f>((E28-C28)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="29" ht="14.4" customHeight="true">
-      <c r="B29" s="43" t="n">
+      <c r="B29" s="354" t="n">
         <v>14.0</v>
       </c>
-      <c r="C29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="G29" s="43" t="s">
-        <v>83</v>
+      <c r="C29" s="355"/>
+      <c r="E29" s="355"/>
+      <c r="G29" s="353" t="n">
+        <f>((E29-C29)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="30" ht="14.4" customHeight="true">
-      <c r="B30" s="43" t="n">
+      <c r="B30" s="354" t="n">
         <v>15.0</v>
       </c>
-      <c r="C30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="G30" s="43" t="s">
-        <v>83</v>
+      <c r="C30" s="355"/>
+      <c r="E30" s="355"/>
+      <c r="G30" s="353" t="n">
+        <f>((E30-C30)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="31" ht="14.4" customHeight="true">
-      <c r="B31" s="43" t="n">
+      <c r="B31" s="354" t="n">
         <v>16.0</v>
       </c>
-      <c r="C31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="G31" s="43" t="s">
-        <v>83</v>
+      <c r="C31" s="355"/>
+      <c r="E31" s="355"/>
+      <c r="G31" s="353" t="n">
+        <f>((E31-C31)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="32" ht="14.4" customHeight="true">
-      <c r="B32" s="43" t="n">
+      <c r="B32" s="354" t="n">
         <v>17.0</v>
       </c>
-      <c r="C32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="G32" s="43" t="s">
-        <v>83</v>
+      <c r="C32" s="355"/>
+      <c r="E32" s="355"/>
+      <c r="G32" s="353" t="n">
+        <f>((E32-C32)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="33" ht="14.4" customHeight="true">
@@ -8150,53 +8163,58 @@
       </c>
     </row>
     <row r="35" ht="14.4" customHeight="true">
-      <c r="B35" s="46" t="n">
+      <c r="B35" s="354" t="n">
         <v>20.0</v>
       </c>
-      <c r="C35" s="46"/>
-      <c r="E35" s="46"/>
-      <c r="G35" s="46" t="s">
-        <v>83</v>
+      <c r="C35" s="355"/>
+      <c r="E35" s="355"/>
+      <c r="G35" s="353" t="n">
+        <f>((E35-C35)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="36" ht="14.4" customHeight="true">
-      <c r="B36" s="46" t="n">
+      <c r="B36" s="354" t="n">
         <v>21.0</v>
       </c>
-      <c r="C36" s="46"/>
-      <c r="E36" s="46"/>
-      <c r="G36" s="46" t="s">
-        <v>83</v>
+      <c r="C36" s="355"/>
+      <c r="E36" s="355"/>
+      <c r="G36" s="353" t="n">
+        <f>((E36-C36)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="37" ht="14.4" customHeight="true">
-      <c r="B37" s="46" t="n">
+      <c r="B37" s="354" t="n">
         <v>22.0</v>
       </c>
-      <c r="C37" s="46"/>
-      <c r="E37" s="46"/>
-      <c r="G37" s="46" t="s">
-        <v>83</v>
+      <c r="C37" s="355"/>
+      <c r="E37" s="355"/>
+      <c r="G37" s="353" t="n">
+        <f>((E37-C37)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="38" ht="14.4" customHeight="true">
-      <c r="B38" s="46" t="n">
+      <c r="B38" s="354" t="n">
         <v>23.0</v>
       </c>
-      <c r="C38" s="46"/>
-      <c r="E38" s="46"/>
-      <c r="G38" s="46" t="s">
-        <v>83</v>
+      <c r="C38" s="355"/>
+      <c r="E38" s="355"/>
+      <c r="G38" s="353" t="n">
+        <f>((E38-C38)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="39" ht="14.4" customHeight="true">
-      <c r="B39" s="46" t="n">
+      <c r="B39" s="354" t="n">
         <v>24.0</v>
       </c>
-      <c r="C39" s="46"/>
-      <c r="E39" s="46"/>
-      <c r="G39" s="46" t="s">
-        <v>83</v>
+      <c r="C39" s="355"/>
+      <c r="E39" s="355"/>
+      <c r="G39" s="353" t="n">
+        <f>((E39-C39)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="40" ht="14.4" customHeight="true">
@@ -8220,43 +8238,47 @@
       </c>
     </row>
     <row r="42" ht="14.4" customHeight="true">
-      <c r="B42" s="56" t="n">
+      <c r="B42" s="354" t="n">
         <v>27.0</v>
       </c>
-      <c r="C42" s="56"/>
-      <c r="E42" s="56"/>
-      <c r="G42" s="56" t="s">
-        <v>83</v>
+      <c r="C42" s="355"/>
+      <c r="E42" s="355"/>
+      <c r="G42" s="353" t="n">
+        <f>((E42-C42)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="43" ht="14.4" customHeight="true">
-      <c r="B43" s="56" t="n">
+      <c r="B43" s="354" t="n">
         <v>28.0</v>
       </c>
-      <c r="C43" s="56"/>
-      <c r="E43" s="56"/>
-      <c r="G43" s="56" t="s">
-        <v>83</v>
+      <c r="C43" s="355"/>
+      <c r="E43" s="355"/>
+      <c r="G43" s="353" t="n">
+        <f>((E43-C43)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="44" ht="14.4" customHeight="true">
-      <c r="B44" s="56" t="n">
+      <c r="B44" s="354" t="n">
         <v>29.0</v>
       </c>
-      <c r="C44" s="56"/>
-      <c r="E44" s="56"/>
-      <c r="G44" s="56" t="s">
-        <v>83</v>
+      <c r="C44" s="355"/>
+      <c r="E44" s="355"/>
+      <c r="G44" s="353" t="n">
+        <f>((E44-C44)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="45" ht="14.4" customHeight="true">
-      <c r="B45" s="57" t="n">
+      <c r="B45" s="354" t="n">
         <v>30.0</v>
       </c>
-      <c r="C45" s="57"/>
-      <c r="E45" s="57"/>
-      <c r="G45" s="57" t="s">
-        <v>83</v>
+      <c r="C45" s="355"/>
+      <c r="E45" s="355"/>
+      <c r="G45" s="353" t="n">
+        <f>((E45-C45)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="46"/>
@@ -8511,13 +8533,14 @@
       <c r="G15" s="382"/>
     </row>
     <row r="16" ht="14.4" customHeight="true">
-      <c r="B16" s="29" t="n">
+      <c r="B16" s="383" t="n">
         <v>1.0</v>
       </c>
-      <c r="C16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="G16" s="29" t="s">
-        <v>83</v>
+      <c r="C16" s="384"/>
+      <c r="E16" s="384"/>
+      <c r="G16" s="382" t="n">
+        <f>((E16-C16)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="17" ht="14.4" customHeight="true">
@@ -8541,53 +8564,58 @@
       </c>
     </row>
     <row r="19" ht="14.4" customHeight="true">
-      <c r="B19" s="36" t="n">
+      <c r="B19" s="383" t="n">
         <v>4.0</v>
       </c>
-      <c r="C19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="G19" s="36" t="s">
-        <v>83</v>
+      <c r="C19" s="384"/>
+      <c r="E19" s="384"/>
+      <c r="G19" s="382" t="n">
+        <f>((E19-C19)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="20" ht="14.4" customHeight="true">
-      <c r="B20" s="36" t="n">
+      <c r="B20" s="383" t="n">
         <v>5.0</v>
       </c>
-      <c r="C20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="G20" s="36" t="s">
-        <v>83</v>
+      <c r="C20" s="384"/>
+      <c r="E20" s="384"/>
+      <c r="G20" s="382" t="n">
+        <f>((E20-C20)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="21" ht="14.4" customHeight="true">
-      <c r="B21" s="36" t="n">
+      <c r="B21" s="383" t="n">
         <v>6.0</v>
       </c>
-      <c r="C21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="G21" s="36" t="s">
-        <v>83</v>
+      <c r="C21" s="384"/>
+      <c r="E21" s="384"/>
+      <c r="G21" s="382" t="n">
+        <f>((E21-C21)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="22" ht="14.4" customHeight="true">
-      <c r="B22" s="36" t="n">
+      <c r="B22" s="383" t="n">
         <v>7.0</v>
       </c>
-      <c r="C22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="G22" s="36" t="s">
-        <v>83</v>
+      <c r="C22" s="384"/>
+      <c r="E22" s="384"/>
+      <c r="G22" s="382" t="n">
+        <f>((E22-C22)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="23" ht="14.4" customHeight="true">
-      <c r="B23" s="36" t="n">
+      <c r="B23" s="383" t="n">
         <v>8.0</v>
       </c>
-      <c r="C23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="G23" s="36" t="s">
-        <v>83</v>
+      <c r="C23" s="384"/>
+      <c r="E23" s="384"/>
+      <c r="G23" s="382" t="n">
+        <f>((E23-C23)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="24" ht="14.4" customHeight="true">
@@ -8611,13 +8639,14 @@
       </c>
     </row>
     <row r="26" ht="14.4" customHeight="true">
-      <c r="B26" s="43" t="n">
+      <c r="B26" s="383" t="n">
         <v>11.0</v>
       </c>
-      <c r="C26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="G26" s="43" t="s">
-        <v>83</v>
+      <c r="C26" s="384"/>
+      <c r="E26" s="384"/>
+      <c r="G26" s="382" t="n">
+        <f>((E26-C26)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="27" ht="14.4" customHeight="true">
@@ -8631,33 +8660,36 @@
       </c>
     </row>
     <row r="28" ht="14.4" customHeight="true">
-      <c r="B28" s="43" t="n">
+      <c r="B28" s="383" t="n">
         <v>13.0</v>
       </c>
-      <c r="C28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="G28" s="43" t="s">
-        <v>83</v>
+      <c r="C28" s="384"/>
+      <c r="E28" s="384"/>
+      <c r="G28" s="382" t="n">
+        <f>((E28-C28)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="29" ht="14.4" customHeight="true">
-      <c r="B29" s="43" t="n">
+      <c r="B29" s="383" t="n">
         <v>14.0</v>
       </c>
-      <c r="C29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="G29" s="43" t="s">
-        <v>83</v>
+      <c r="C29" s="384"/>
+      <c r="E29" s="384"/>
+      <c r="G29" s="382" t="n">
+        <f>((E29-C29)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="30" ht="14.4" customHeight="true">
-      <c r="B30" s="43" t="n">
+      <c r="B30" s="383" t="n">
         <v>15.0</v>
       </c>
-      <c r="C30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="G30" s="43" t="s">
-        <v>83</v>
+      <c r="C30" s="384"/>
+      <c r="E30" s="384"/>
+      <c r="G30" s="382" t="n">
+        <f>((E30-C30)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="31" ht="14.4" customHeight="true">
@@ -8681,53 +8713,58 @@
       </c>
     </row>
     <row r="33" ht="14.4" customHeight="true">
-      <c r="B33" s="43" t="n">
+      <c r="B33" s="383" t="n">
         <v>18.0</v>
       </c>
-      <c r="C33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="G33" s="43" t="s">
-        <v>83</v>
+      <c r="C33" s="384"/>
+      <c r="E33" s="384"/>
+      <c r="G33" s="382" t="n">
+        <f>((E33-C33)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="34" ht="14.4" customHeight="true">
-      <c r="B34" s="43" t="n">
+      <c r="B34" s="383" t="n">
         <v>19.0</v>
       </c>
-      <c r="C34" s="43"/>
-      <c r="E34" s="43"/>
-      <c r="G34" s="43" t="s">
-        <v>83</v>
+      <c r="C34" s="384"/>
+      <c r="E34" s="384"/>
+      <c r="G34" s="382" t="n">
+        <f>((E34-C34)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="35" ht="14.4" customHeight="true">
-      <c r="B35" s="43" t="n">
+      <c r="B35" s="383" t="n">
         <v>20.0</v>
       </c>
-      <c r="C35" s="43"/>
-      <c r="E35" s="43"/>
-      <c r="G35" s="43" t="s">
-        <v>83</v>
+      <c r="C35" s="384"/>
+      <c r="E35" s="384"/>
+      <c r="G35" s="382" t="n">
+        <f>((E35-C35)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="36" ht="14.4" customHeight="true">
-      <c r="B36" s="43" t="n">
+      <c r="B36" s="383" t="n">
         <v>21.0</v>
       </c>
-      <c r="C36" s="43"/>
-      <c r="E36" s="43"/>
-      <c r="G36" s="43" t="s">
-        <v>83</v>
+      <c r="C36" s="384"/>
+      <c r="E36" s="384"/>
+      <c r="G36" s="382" t="n">
+        <f>((E36-C36)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="37" ht="14.4" customHeight="true">
-      <c r="B37" s="43" t="n">
+      <c r="B37" s="383" t="n">
         <v>22.0</v>
       </c>
-      <c r="C37" s="43"/>
-      <c r="E37" s="43"/>
-      <c r="G37" s="43" t="s">
-        <v>83</v>
+      <c r="C37" s="384"/>
+      <c r="E37" s="384"/>
+      <c r="G37" s="382" t="n">
+        <f>((E37-C37)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="38" ht="14.4" customHeight="true">
@@ -8751,53 +8788,58 @@
       </c>
     </row>
     <row r="40" ht="14.4" customHeight="true">
-      <c r="B40" s="46" t="n">
+      <c r="B40" s="383" t="n">
         <v>25.0</v>
       </c>
-      <c r="C40" s="46"/>
-      <c r="E40" s="46"/>
-      <c r="G40" s="46" t="s">
-        <v>83</v>
+      <c r="C40" s="384"/>
+      <c r="E40" s="384"/>
+      <c r="G40" s="382" t="n">
+        <f>((E40-C40)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="41" ht="14.4" customHeight="true">
-      <c r="B41" s="46" t="n">
+      <c r="B41" s="383" t="n">
         <v>26.0</v>
       </c>
-      <c r="C41" s="46"/>
-      <c r="E41" s="46"/>
-      <c r="G41" s="46" t="s">
-        <v>83</v>
+      <c r="C41" s="384"/>
+      <c r="E41" s="384"/>
+      <c r="G41" s="382" t="n">
+        <f>((E41-C41)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="42" ht="14.4" customHeight="true">
-      <c r="B42" s="46" t="n">
+      <c r="B42" s="383" t="n">
         <v>27.0</v>
       </c>
-      <c r="C42" s="46"/>
-      <c r="E42" s="46"/>
-      <c r="G42" s="46" t="s">
-        <v>83</v>
+      <c r="C42" s="384"/>
+      <c r="E42" s="384"/>
+      <c r="G42" s="382" t="n">
+        <f>((E42-C42)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="43" ht="14.4" customHeight="true">
-      <c r="B43" s="46" t="n">
+      <c r="B43" s="383" t="n">
         <v>28.0</v>
       </c>
-      <c r="C43" s="46"/>
-      <c r="E43" s="46"/>
-      <c r="G43" s="46" t="s">
-        <v>83</v>
+      <c r="C43" s="384"/>
+      <c r="E43" s="384"/>
+      <c r="G43" s="382" t="n">
+        <f>((E43-C43)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="44" ht="14.4" customHeight="true">
-      <c r="B44" s="46" t="n">
+      <c r="B44" s="383" t="n">
         <v>29.0</v>
       </c>
-      <c r="C44" s="46"/>
-      <c r="E44" s="46"/>
-      <c r="G44" s="46" t="s">
-        <v>83</v>
+      <c r="C44" s="384"/>
+      <c r="E44" s="384"/>
+      <c r="G44" s="382" t="n">
+        <f>((E44-C44)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="45" ht="14.4" customHeight="true">
@@ -9081,43 +9123,47 @@
       </c>
     </row>
     <row r="17" ht="14.4" customHeight="true">
-      <c r="B17" s="30" t="n">
+      <c r="B17" s="412" t="n">
         <v>2.0</v>
       </c>
-      <c r="C17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="G17" s="30" t="s">
-        <v>83</v>
+      <c r="C17" s="413"/>
+      <c r="E17" s="413"/>
+      <c r="G17" s="411" t="n">
+        <f>((E17-C17)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="18" ht="14.4" customHeight="true">
-      <c r="B18" s="30" t="n">
+      <c r="B18" s="412" t="n">
         <v>3.0</v>
       </c>
-      <c r="C18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="G18" s="30" t="s">
-        <v>83</v>
+      <c r="C18" s="413"/>
+      <c r="E18" s="413"/>
+      <c r="G18" s="411" t="n">
+        <f>((E18-C18)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="19" ht="14.4" customHeight="true">
-      <c r="B19" s="30" t="n">
+      <c r="B19" s="412" t="n">
         <v>4.0</v>
       </c>
-      <c r="C19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="G19" s="30" t="s">
-        <v>83</v>
+      <c r="C19" s="413"/>
+      <c r="E19" s="413"/>
+      <c r="G19" s="411" t="n">
+        <f>((E19-C19)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="20" ht="14.4" customHeight="true">
-      <c r="B20" s="30" t="n">
+      <c r="B20" s="412" t="n">
         <v>5.0</v>
       </c>
-      <c r="C20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="G20" s="30" t="s">
-        <v>83</v>
+      <c r="C20" s="413"/>
+      <c r="E20" s="413"/>
+      <c r="G20" s="411" t="n">
+        <f>((E20-C20)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="21" ht="14.4" customHeight="true">
@@ -9141,53 +9187,58 @@
       </c>
     </row>
     <row r="23" ht="14.4" customHeight="true">
-      <c r="B23" s="36" t="n">
+      <c r="B23" s="412" t="n">
         <v>8.0</v>
       </c>
-      <c r="C23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="G23" s="36" t="s">
-        <v>83</v>
+      <c r="C23" s="413"/>
+      <c r="E23" s="413"/>
+      <c r="G23" s="411" t="n">
+        <f>((E23-C23)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="24" ht="14.4" customHeight="true">
-      <c r="B24" s="36" t="n">
+      <c r="B24" s="412" t="n">
         <v>9.0</v>
       </c>
-      <c r="C24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="G24" s="36" t="s">
-        <v>83</v>
+      <c r="C24" s="413"/>
+      <c r="E24" s="413"/>
+      <c r="G24" s="411" t="n">
+        <f>((E24-C24)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="25" ht="14.4" customHeight="true">
-      <c r="B25" s="36" t="n">
+      <c r="B25" s="412" t="n">
         <v>10.0</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="G25" s="36" t="s">
-        <v>83</v>
+      <c r="C25" s="413"/>
+      <c r="E25" s="413"/>
+      <c r="G25" s="411" t="n">
+        <f>((E25-C25)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="26" ht="14.4" customHeight="true">
-      <c r="B26" s="36" t="n">
+      <c r="B26" s="412" t="n">
         <v>11.0</v>
       </c>
-      <c r="C26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="G26" s="36" t="s">
-        <v>83</v>
+      <c r="C26" s="413"/>
+      <c r="E26" s="413"/>
+      <c r="G26" s="411" t="n">
+        <f>((E26-C26)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="27" ht="14.4" customHeight="true">
-      <c r="B27" s="36" t="n">
+      <c r="B27" s="412" t="n">
         <v>12.0</v>
       </c>
-      <c r="C27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="G27" s="36" t="s">
-        <v>83</v>
+      <c r="C27" s="413"/>
+      <c r="E27" s="413"/>
+      <c r="G27" s="411" t="n">
+        <f>((E27-C27)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="28" ht="14.4" customHeight="true">
@@ -9211,53 +9262,58 @@
       </c>
     </row>
     <row r="30" ht="14.4" customHeight="true">
-      <c r="B30" s="43" t="n">
+      <c r="B30" s="412" t="n">
         <v>15.0</v>
       </c>
-      <c r="C30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="G30" s="43" t="s">
-        <v>83</v>
+      <c r="C30" s="413"/>
+      <c r="E30" s="413"/>
+      <c r="G30" s="411" t="n">
+        <f>((E30-C30)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="31" ht="14.4" customHeight="true">
-      <c r="B31" s="43" t="n">
+      <c r="B31" s="412" t="n">
         <v>16.0</v>
       </c>
-      <c r="C31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="G31" s="43" t="s">
-        <v>83</v>
+      <c r="C31" s="413"/>
+      <c r="E31" s="413"/>
+      <c r="G31" s="411" t="n">
+        <f>((E31-C31)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="32" ht="14.4" customHeight="true">
-      <c r="B32" s="43" t="n">
+      <c r="B32" s="412" t="n">
         <v>17.0</v>
       </c>
-      <c r="C32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="G32" s="43" t="s">
-        <v>83</v>
+      <c r="C32" s="413"/>
+      <c r="E32" s="413"/>
+      <c r="G32" s="411" t="n">
+        <f>((E32-C32)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="33" ht="14.4" customHeight="true">
-      <c r="B33" s="43" t="n">
+      <c r="B33" s="412" t="n">
         <v>18.0</v>
       </c>
-      <c r="C33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="G33" s="43" t="s">
-        <v>83</v>
+      <c r="C33" s="413"/>
+      <c r="E33" s="413"/>
+      <c r="G33" s="411" t="n">
+        <f>((E33-C33)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="34" ht="14.4" customHeight="true">
-      <c r="B34" s="43" t="n">
+      <c r="B34" s="412" t="n">
         <v>19.0</v>
       </c>
-      <c r="C34" s="43"/>
-      <c r="E34" s="43"/>
-      <c r="G34" s="43" t="s">
-        <v>83</v>
+      <c r="C34" s="413"/>
+      <c r="E34" s="413"/>
+      <c r="G34" s="411" t="n">
+        <f>((E34-C34)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="35" ht="14.4" customHeight="true">
@@ -9281,53 +9337,58 @@
       </c>
     </row>
     <row r="37" ht="14.4" customHeight="true">
-      <c r="B37" s="46" t="n">
+      <c r="B37" s="412" t="n">
         <v>22.0</v>
       </c>
-      <c r="C37" s="46"/>
-      <c r="E37" s="46"/>
-      <c r="G37" s="46" t="s">
-        <v>83</v>
+      <c r="C37" s="413"/>
+      <c r="E37" s="413"/>
+      <c r="G37" s="411" t="n">
+        <f>((E37-C37)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="38" ht="14.4" customHeight="true">
-      <c r="B38" s="46" t="n">
+      <c r="B38" s="412" t="n">
         <v>23.0</v>
       </c>
-      <c r="C38" s="46"/>
-      <c r="E38" s="46"/>
-      <c r="G38" s="46" t="s">
-        <v>83</v>
+      <c r="C38" s="413"/>
+      <c r="E38" s="413"/>
+      <c r="G38" s="411" t="n">
+        <f>((E38-C38)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="39" ht="14.4" customHeight="true">
-      <c r="B39" s="46" t="n">
+      <c r="B39" s="412" t="n">
         <v>24.0</v>
       </c>
-      <c r="C39" s="46"/>
-      <c r="E39" s="46"/>
-      <c r="G39" s="46" t="s">
-        <v>83</v>
+      <c r="C39" s="413"/>
+      <c r="E39" s="413"/>
+      <c r="G39" s="411" t="n">
+        <f>((E39-C39)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="40" ht="14.4" customHeight="true">
-      <c r="B40" s="46" t="n">
+      <c r="B40" s="412" t="n">
         <v>25.0</v>
       </c>
-      <c r="C40" s="46"/>
-      <c r="E40" s="46"/>
-      <c r="G40" s="46" t="s">
-        <v>83</v>
+      <c r="C40" s="413"/>
+      <c r="E40" s="413"/>
+      <c r="G40" s="411" t="n">
+        <f>((E40-C40)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="41" ht="14.4" customHeight="true">
-      <c r="B41" s="46" t="n">
+      <c r="B41" s="412" t="n">
         <v>26.0</v>
       </c>
-      <c r="C41" s="46"/>
-      <c r="E41" s="46"/>
-      <c r="G41" s="46" t="s">
-        <v>83</v>
+      <c r="C41" s="413"/>
+      <c r="E41" s="413"/>
+      <c r="G41" s="411" t="n">
+        <f>((E41-C41)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="42" ht="14.4" customHeight="true">
@@ -9351,23 +9412,25 @@
       </c>
     </row>
     <row r="44" ht="14.4" customHeight="true">
-      <c r="B44" s="56" t="n">
+      <c r="B44" s="412" t="n">
         <v>29.0</v>
       </c>
-      <c r="C44" s="56"/>
-      <c r="E44" s="56"/>
-      <c r="G44" s="56" t="s">
-        <v>83</v>
+      <c r="C44" s="413"/>
+      <c r="E44" s="413"/>
+      <c r="G44" s="411" t="n">
+        <f>((E44-C44)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="45" ht="14.4" customHeight="true">
-      <c r="B45" s="57" t="n">
+      <c r="B45" s="412" t="n">
         <v>30.0</v>
       </c>
-      <c r="C45" s="57"/>
-      <c r="E45" s="57"/>
-      <c r="G45" s="57" t="s">
-        <v>83</v>
+      <c r="C45" s="413"/>
+      <c r="E45" s="413"/>
+      <c r="G45" s="411" t="n">
+        <f>((E45-C45)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="46"/>
@@ -9622,33 +9685,36 @@
       <c r="G15" s="440"/>
     </row>
     <row r="16" ht="14.4" customHeight="true">
-      <c r="B16" s="29" t="n">
+      <c r="B16" s="441" t="n">
         <v>1.0</v>
       </c>
-      <c r="C16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="G16" s="29" t="s">
-        <v>83</v>
+      <c r="C16" s="442"/>
+      <c r="E16" s="442"/>
+      <c r="G16" s="440" t="n">
+        <f>((E16-C16)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="17" ht="14.4" customHeight="true">
-      <c r="B17" s="30" t="n">
+      <c r="B17" s="441" t="n">
         <v>2.0</v>
       </c>
-      <c r="C17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="G17" s="30" t="s">
-        <v>83</v>
+      <c r="C17" s="442"/>
+      <c r="E17" s="442"/>
+      <c r="G17" s="440" t="n">
+        <f>((E17-C17)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="18" ht="14.4" customHeight="true">
-      <c r="B18" s="30" t="n">
+      <c r="B18" s="441" t="n">
         <v>3.0</v>
       </c>
-      <c r="C18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="G18" s="30" t="s">
-        <v>83</v>
+      <c r="C18" s="442"/>
+      <c r="E18" s="442"/>
+      <c r="G18" s="440" t="n">
+        <f>((E18-C18)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="19" ht="14.4" customHeight="true">
@@ -9682,13 +9748,14 @@
       </c>
     </row>
     <row r="22" ht="14.4" customHeight="true">
-      <c r="B22" s="36" t="n">
+      <c r="B22" s="441" t="n">
         <v>7.0</v>
       </c>
-      <c r="C22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="G22" s="36" t="s">
-        <v>83</v>
+      <c r="C22" s="442"/>
+      <c r="E22" s="442"/>
+      <c r="G22" s="440" t="n">
+        <f>((E22-C22)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="23" ht="14.4" customHeight="true">
@@ -9702,23 +9769,25 @@
       </c>
     </row>
     <row r="24" ht="14.4" customHeight="true">
-      <c r="B24" s="36" t="n">
+      <c r="B24" s="441" t="n">
         <v>9.0</v>
       </c>
-      <c r="C24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="G24" s="36" t="s">
-        <v>83</v>
+      <c r="C24" s="442"/>
+      <c r="E24" s="442"/>
+      <c r="G24" s="440" t="n">
+        <f>((E24-C24)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="25" ht="14.4" customHeight="true">
-      <c r="B25" s="36" t="n">
+      <c r="B25" s="441" t="n">
         <v>10.0</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="G25" s="36" t="s">
-        <v>83</v>
+      <c r="C25" s="442"/>
+      <c r="E25" s="442"/>
+      <c r="G25" s="440" t="n">
+        <f>((E25-C25)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="26" ht="14.4" customHeight="true">
@@ -9742,53 +9811,58 @@
       </c>
     </row>
     <row r="28" ht="14.4" customHeight="true">
-      <c r="B28" s="43" t="n">
+      <c r="B28" s="441" t="n">
         <v>13.0</v>
       </c>
-      <c r="C28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="G28" s="43" t="s">
-        <v>83</v>
+      <c r="C28" s="442"/>
+      <c r="E28" s="442"/>
+      <c r="G28" s="440" t="n">
+        <f>((E28-C28)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="29" ht="14.4" customHeight="true">
-      <c r="B29" s="43" t="n">
+      <c r="B29" s="441" t="n">
         <v>14.0</v>
       </c>
-      <c r="C29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="G29" s="43" t="s">
-        <v>83</v>
+      <c r="C29" s="442"/>
+      <c r="E29" s="442"/>
+      <c r="G29" s="440" t="n">
+        <f>((E29-C29)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="30" ht="14.4" customHeight="true">
-      <c r="B30" s="43" t="n">
+      <c r="B30" s="441" t="n">
         <v>15.0</v>
       </c>
-      <c r="C30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="G30" s="43" t="s">
-        <v>83</v>
+      <c r="C30" s="442"/>
+      <c r="E30" s="442"/>
+      <c r="G30" s="440" t="n">
+        <f>((E30-C30)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="31" ht="14.4" customHeight="true">
-      <c r="B31" s="43" t="n">
+      <c r="B31" s="441" t="n">
         <v>16.0</v>
       </c>
-      <c r="C31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="G31" s="43" t="s">
-        <v>83</v>
+      <c r="C31" s="442"/>
+      <c r="E31" s="442"/>
+      <c r="G31" s="440" t="n">
+        <f>((E31-C31)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="32" ht="14.4" customHeight="true">
-      <c r="B32" s="43" t="n">
+      <c r="B32" s="441" t="n">
         <v>17.0</v>
       </c>
-      <c r="C32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="G32" s="43" t="s">
-        <v>83</v>
+      <c r="C32" s="442"/>
+      <c r="E32" s="442"/>
+      <c r="G32" s="440" t="n">
+        <f>((E32-C32)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="33" ht="14.4" customHeight="true">
@@ -9812,53 +9886,58 @@
       </c>
     </row>
     <row r="35" ht="14.4" customHeight="true">
-      <c r="B35" s="46" t="n">
+      <c r="B35" s="441" t="n">
         <v>20.0</v>
       </c>
-      <c r="C35" s="46"/>
-      <c r="E35" s="46"/>
-      <c r="G35" s="46" t="s">
-        <v>83</v>
+      <c r="C35" s="442"/>
+      <c r="E35" s="442"/>
+      <c r="G35" s="440" t="n">
+        <f>((E35-C35)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="36" ht="14.4" customHeight="true">
-      <c r="B36" s="46" t="n">
+      <c r="B36" s="441" t="n">
         <v>21.0</v>
       </c>
-      <c r="C36" s="46"/>
-      <c r="E36" s="46"/>
-      <c r="G36" s="46" t="s">
-        <v>83</v>
+      <c r="C36" s="442"/>
+      <c r="E36" s="442"/>
+      <c r="G36" s="440" t="n">
+        <f>((E36-C36)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="37" ht="14.4" customHeight="true">
-      <c r="B37" s="46" t="n">
+      <c r="B37" s="441" t="n">
         <v>22.0</v>
       </c>
-      <c r="C37" s="46"/>
-      <c r="E37" s="46"/>
-      <c r="G37" s="46" t="s">
-        <v>83</v>
+      <c r="C37" s="442"/>
+      <c r="E37" s="442"/>
+      <c r="G37" s="440" t="n">
+        <f>((E37-C37)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="38" ht="14.4" customHeight="true">
-      <c r="B38" s="46" t="n">
+      <c r="B38" s="441" t="n">
         <v>23.0</v>
       </c>
-      <c r="C38" s="46"/>
-      <c r="E38" s="46"/>
-      <c r="G38" s="46" t="s">
-        <v>83</v>
+      <c r="C38" s="442"/>
+      <c r="E38" s="442"/>
+      <c r="G38" s="440" t="n">
+        <f>((E38-C38)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="39" ht="14.4" customHeight="true">
-      <c r="B39" s="46" t="n">
+      <c r="B39" s="441" t="n">
         <v>24.0</v>
       </c>
-      <c r="C39" s="46"/>
-      <c r="E39" s="46"/>
-      <c r="G39" s="46" t="s">
-        <v>83</v>
+      <c r="C39" s="442"/>
+      <c r="E39" s="442"/>
+      <c r="G39" s="440" t="n">
+        <f>((E39-C39)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="40" ht="14.4" customHeight="true">
@@ -9882,53 +9961,58 @@
       </c>
     </row>
     <row r="42" ht="14.4" customHeight="true">
-      <c r="B42" s="56" t="n">
+      <c r="B42" s="441" t="n">
         <v>27.0</v>
       </c>
-      <c r="C42" s="56"/>
-      <c r="E42" s="56"/>
-      <c r="G42" s="56" t="s">
-        <v>83</v>
+      <c r="C42" s="442"/>
+      <c r="E42" s="442"/>
+      <c r="G42" s="440" t="n">
+        <f>((E42-C42)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="43" ht="14.4" customHeight="true">
-      <c r="B43" s="56" t="n">
+      <c r="B43" s="441" t="n">
         <v>28.0</v>
       </c>
-      <c r="C43" s="56"/>
-      <c r="E43" s="56"/>
-      <c r="G43" s="56" t="s">
-        <v>83</v>
+      <c r="C43" s="442"/>
+      <c r="E43" s="442"/>
+      <c r="G43" s="440" t="n">
+        <f>((E43-C43)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="44" ht="14.4" customHeight="true">
-      <c r="B44" s="56" t="n">
+      <c r="B44" s="441" t="n">
         <v>29.0</v>
       </c>
-      <c r="C44" s="56"/>
-      <c r="E44" s="56"/>
-      <c r="G44" s="56" t="s">
-        <v>83</v>
+      <c r="C44" s="442"/>
+      <c r="E44" s="442"/>
+      <c r="G44" s="440" t="n">
+        <f>((E44-C44)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="45" ht="14.4" customHeight="true">
-      <c r="B45" s="56" t="n">
+      <c r="B45" s="441" t="n">
         <v>30.0</v>
       </c>
-      <c r="C45" s="56"/>
-      <c r="E45" s="56"/>
-      <c r="G45" s="56" t="s">
-        <v>83</v>
+      <c r="C45" s="442"/>
+      <c r="E45" s="442"/>
+      <c r="G45" s="440" t="n">
+        <f>((E45-C45)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="46" ht="14.4" customHeight="true">
-      <c r="B46" s="57" t="n">
+      <c r="B46" s="441" t="n">
         <v>31.0</v>
       </c>
-      <c r="C46" s="57"/>
-      <c r="E46" s="57"/>
-      <c r="G46" s="57" t="s">
-        <v>83</v>
+      <c r="C46" s="442"/>
+      <c r="E46" s="442"/>
+      <c r="G46" s="440" t="n">
+        <f>((E46-C46)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="47" ht="14.4" customHeight="true">
@@ -10227,23 +10311,25 @@
       </c>
     </row>
     <row r="19" ht="14.4" customHeight="true">
-      <c r="B19" s="33" t="n">
+      <c r="B19" s="113" t="n">
         <v>4.0</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="G19" s="33" t="s">
-        <v>83</v>
+      <c r="C19" s="114"/>
+      <c r="E19" s="114"/>
+      <c r="G19" s="112" t="n">
+        <f>((E19-C19)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="20" ht="14.4" customHeight="true">
-      <c r="B20" s="33" t="n">
+      <c r="B20" s="113" t="n">
         <v>5.0</v>
       </c>
-      <c r="C20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="G20" s="33" t="s">
-        <v>83</v>
+      <c r="C20" s="114"/>
+      <c r="E20" s="114"/>
+      <c r="G20" s="112" t="n">
+        <f>((E20-C20)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="21" ht="14.4" customHeight="true">
@@ -10257,23 +10343,25 @@
       </c>
     </row>
     <row r="22" ht="14.4" customHeight="true">
-      <c r="B22" s="33" t="n">
+      <c r="B22" s="113" t="n">
         <v>7.0</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="G22" s="33" t="s">
-        <v>83</v>
+      <c r="C22" s="114"/>
+      <c r="E22" s="114"/>
+      <c r="G22" s="112" t="n">
+        <f>((E22-C22)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="23" ht="14.4" customHeight="true">
-      <c r="B23" s="33" t="n">
+      <c r="B23" s="113" t="n">
         <v>8.0</v>
       </c>
-      <c r="C23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="G23" s="33" t="s">
-        <v>83</v>
+      <c r="C23" s="114"/>
+      <c r="E23" s="114"/>
+      <c r="G23" s="112" t="n">
+        <f>((E23-C23)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="24" ht="14.4" customHeight="true">
@@ -10297,53 +10385,58 @@
       </c>
     </row>
     <row r="26" ht="14.4" customHeight="true">
-      <c r="B26" s="40" t="n">
+      <c r="B26" s="113" t="n">
         <v>11.0</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="E26" s="40"/>
-      <c r="G26" s="40" t="s">
-        <v>83</v>
+      <c r="C26" s="114"/>
+      <c r="E26" s="114"/>
+      <c r="G26" s="112" t="n">
+        <f>((E26-C26)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="27" ht="14.4" customHeight="true">
-      <c r="B27" s="40" t="n">
+      <c r="B27" s="113" t="n">
         <v>12.0</v>
       </c>
-      <c r="C27" s="40"/>
-      <c r="E27" s="40"/>
-      <c r="G27" s="40" t="s">
-        <v>83</v>
+      <c r="C27" s="114"/>
+      <c r="E27" s="114"/>
+      <c r="G27" s="112" t="n">
+        <f>((E27-C27)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="28" ht="14.4" customHeight="true">
-      <c r="B28" s="40" t="n">
+      <c r="B28" s="113" t="n">
         <v>13.0</v>
       </c>
-      <c r="C28" s="40"/>
-      <c r="E28" s="40"/>
-      <c r="G28" s="40" t="s">
-        <v>83</v>
+      <c r="C28" s="114"/>
+      <c r="E28" s="114"/>
+      <c r="G28" s="112" t="n">
+        <f>((E28-C28)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="29" ht="14.4" customHeight="true">
-      <c r="B29" s="40" t="n">
+      <c r="B29" s="113" t="n">
         <v>14.0</v>
       </c>
-      <c r="C29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="G29" s="40" t="s">
-        <v>83</v>
+      <c r="C29" s="114"/>
+      <c r="E29" s="114"/>
+      <c r="G29" s="112" t="n">
+        <f>((E29-C29)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="30" ht="14.4" customHeight="true">
-      <c r="B30" s="40" t="n">
+      <c r="B30" s="113" t="n">
         <v>15.0</v>
       </c>
-      <c r="C30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="G30" s="40" t="s">
-        <v>83</v>
+      <c r="C30" s="114"/>
+      <c r="E30" s="114"/>
+      <c r="G30" s="112" t="n">
+        <f>((E30-C30)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="31" ht="14.4" customHeight="true">
@@ -10367,53 +10460,58 @@
       </c>
     </row>
     <row r="33" ht="14.4" customHeight="true">
-      <c r="B33" s="40" t="n">
+      <c r="B33" s="113" t="n">
         <v>18.0</v>
       </c>
-      <c r="C33" s="40"/>
-      <c r="E33" s="40"/>
-      <c r="G33" s="40" t="s">
-        <v>83</v>
+      <c r="C33" s="114"/>
+      <c r="E33" s="114"/>
+      <c r="G33" s="112" t="n">
+        <f>((E33-C33)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="34" ht="14.4" customHeight="true">
-      <c r="B34" s="40" t="n">
+      <c r="B34" s="113" t="n">
         <v>19.0</v>
       </c>
-      <c r="C34" s="40"/>
-      <c r="E34" s="40"/>
-      <c r="G34" s="40" t="s">
-        <v>83</v>
+      <c r="C34" s="114"/>
+      <c r="E34" s="114"/>
+      <c r="G34" s="112" t="n">
+        <f>((E34-C34)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="35" ht="14.4" customHeight="true">
-      <c r="B35" s="40" t="n">
+      <c r="B35" s="113" t="n">
         <v>20.0</v>
       </c>
-      <c r="C35" s="40"/>
-      <c r="E35" s="40"/>
-      <c r="G35" s="40" t="s">
-        <v>83</v>
+      <c r="C35" s="114"/>
+      <c r="E35" s="114"/>
+      <c r="G35" s="112" t="n">
+        <f>((E35-C35)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="36" ht="14.4" customHeight="true">
-      <c r="B36" s="40" t="n">
+      <c r="B36" s="113" t="n">
         <v>21.0</v>
       </c>
-      <c r="C36" s="40"/>
-      <c r="E36" s="40"/>
-      <c r="G36" s="40" t="s">
-        <v>83</v>
+      <c r="C36" s="114"/>
+      <c r="E36" s="114"/>
+      <c r="G36" s="112" t="n">
+        <f>((E36-C36)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="37" ht="14.4" customHeight="true">
-      <c r="B37" s="40" t="n">
+      <c r="B37" s="113" t="n">
         <v>22.0</v>
       </c>
-      <c r="C37" s="40"/>
-      <c r="E37" s="40"/>
-      <c r="G37" s="40" t="s">
-        <v>83</v>
+      <c r="C37" s="114"/>
+      <c r="E37" s="114"/>
+      <c r="G37" s="112" t="n">
+        <f>((E37-C37)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="38" ht="14.4" customHeight="true">
@@ -10437,53 +10535,58 @@
       </c>
     </row>
     <row r="40" ht="14.4" customHeight="true">
-      <c r="B40" s="49" t="n">
+      <c r="B40" s="113" t="n">
         <v>25.0</v>
       </c>
-      <c r="C40" s="49"/>
-      <c r="E40" s="49"/>
-      <c r="G40" s="49" t="s">
-        <v>83</v>
+      <c r="C40" s="114"/>
+      <c r="E40" s="114"/>
+      <c r="G40" s="112" t="n">
+        <f>((E40-C40)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="41" ht="14.4" customHeight="true">
-      <c r="B41" s="49" t="n">
+      <c r="B41" s="113" t="n">
         <v>26.0</v>
       </c>
-      <c r="C41" s="49"/>
-      <c r="E41" s="49"/>
-      <c r="G41" s="49" t="s">
-        <v>83</v>
+      <c r="C41" s="114"/>
+      <c r="E41" s="114"/>
+      <c r="G41" s="112" t="n">
+        <f>((E41-C41)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="42" ht="14.4" customHeight="true">
-      <c r="B42" s="49" t="n">
+      <c r="B42" s="113" t="n">
         <v>27.0</v>
       </c>
-      <c r="C42" s="49"/>
-      <c r="E42" s="49"/>
-      <c r="G42" s="49" t="s">
-        <v>83</v>
+      <c r="C42" s="114"/>
+      <c r="E42" s="114"/>
+      <c r="G42" s="112" t="n">
+        <f>((E42-C42)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="43" ht="14.4" customHeight="true">
-      <c r="B43" s="49" t="n">
+      <c r="B43" s="113" t="n">
         <v>28.0</v>
       </c>
-      <c r="C43" s="49"/>
-      <c r="E43" s="49"/>
-      <c r="G43" s="49" t="s">
-        <v>83</v>
+      <c r="C43" s="114"/>
+      <c r="E43" s="114"/>
+      <c r="G43" s="112" t="n">
+        <f>((E43-C43)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="44" ht="14.4" customHeight="true">
-      <c r="B44" s="49" t="n">
+      <c r="B44" s="113" t="n">
         <v>29.0</v>
       </c>
-      <c r="C44" s="49"/>
-      <c r="E44" s="49"/>
-      <c r="G44" s="49" t="s">
-        <v>83</v>
+      <c r="C44" s="114"/>
+      <c r="E44" s="114"/>
+      <c r="G44" s="112" t="n">
+        <f>((E44-C44)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="45" ht="14.4" customHeight="true">
@@ -10772,53 +10875,58 @@
       <c r="G15" s="143"/>
     </row>
     <row r="16" ht="14.4" customHeight="true">
-      <c r="B16" s="29" t="n">
+      <c r="B16" s="144" t="n">
         <v>1.0</v>
       </c>
-      <c r="C16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="G16" s="29" t="s">
-        <v>83</v>
+      <c r="C16" s="145"/>
+      <c r="E16" s="145"/>
+      <c r="G16" s="143" t="n">
+        <f>((E16-C16)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="17" ht="14.4" customHeight="true">
-      <c r="B17" s="30" t="n">
+      <c r="B17" s="144" t="n">
         <v>2.0</v>
       </c>
-      <c r="C17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="G17" s="30" t="s">
-        <v>83</v>
+      <c r="C17" s="145"/>
+      <c r="E17" s="145"/>
+      <c r="G17" s="143" t="n">
+        <f>((E17-C17)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="18" ht="14.4" customHeight="true">
-      <c r="B18" s="30" t="n">
+      <c r="B18" s="144" t="n">
         <v>3.0</v>
       </c>
-      <c r="C18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="G18" s="30" t="s">
-        <v>83</v>
+      <c r="C18" s="145"/>
+      <c r="E18" s="145"/>
+      <c r="G18" s="143" t="n">
+        <f>((E18-C18)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="19" ht="14.4" customHeight="true">
-      <c r="B19" s="30" t="n">
+      <c r="B19" s="144" t="n">
         <v>4.0</v>
       </c>
-      <c r="C19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="G19" s="30" t="s">
-        <v>83</v>
+      <c r="C19" s="145"/>
+      <c r="E19" s="145"/>
+      <c r="G19" s="143" t="n">
+        <f>((E19-C19)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="20" ht="14.4" customHeight="true">
-      <c r="B20" s="30" t="n">
+      <c r="B20" s="144" t="n">
         <v>5.0</v>
       </c>
-      <c r="C20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="G20" s="30" t="s">
-        <v>83</v>
+      <c r="C20" s="145"/>
+      <c r="E20" s="145"/>
+      <c r="G20" s="143" t="n">
+        <f>((E20-C20)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="21" ht="14.4" customHeight="true">
@@ -10842,53 +10950,58 @@
       </c>
     </row>
     <row r="23" ht="14.4" customHeight="true">
-      <c r="B23" s="36" t="n">
+      <c r="B23" s="144" t="n">
         <v>8.0</v>
       </c>
-      <c r="C23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="G23" s="36" t="s">
-        <v>83</v>
+      <c r="C23" s="145"/>
+      <c r="E23" s="145"/>
+      <c r="G23" s="143" t="n">
+        <f>((E23-C23)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="24" ht="14.4" customHeight="true">
-      <c r="B24" s="36" t="n">
+      <c r="B24" s="144" t="n">
         <v>9.0</v>
       </c>
-      <c r="C24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="G24" s="36" t="s">
-        <v>83</v>
+      <c r="C24" s="145"/>
+      <c r="E24" s="145"/>
+      <c r="G24" s="143" t="n">
+        <f>((E24-C24)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="25" ht="14.4" customHeight="true">
-      <c r="B25" s="36" t="n">
+      <c r="B25" s="144" t="n">
         <v>10.0</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="G25" s="36" t="s">
-        <v>83</v>
+      <c r="C25" s="145"/>
+      <c r="E25" s="145"/>
+      <c r="G25" s="143" t="n">
+        <f>((E25-C25)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="26" ht="14.4" customHeight="true">
-      <c r="B26" s="36" t="n">
+      <c r="B26" s="144" t="n">
         <v>11.0</v>
       </c>
-      <c r="C26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="G26" s="36" t="s">
-        <v>83</v>
+      <c r="C26" s="145"/>
+      <c r="E26" s="145"/>
+      <c r="G26" s="143" t="n">
+        <f>((E26-C26)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="27" ht="14.4" customHeight="true">
-      <c r="B27" s="36" t="n">
+      <c r="B27" s="144" t="n">
         <v>12.0</v>
       </c>
-      <c r="C27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="G27" s="36" t="s">
-        <v>83</v>
+      <c r="C27" s="145"/>
+      <c r="E27" s="145"/>
+      <c r="G27" s="143" t="n">
+        <f>((E27-C27)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="28" ht="14.4" customHeight="true">
@@ -10912,53 +11025,58 @@
       </c>
     </row>
     <row r="30" ht="14.4" customHeight="true">
-      <c r="B30" s="43" t="n">
+      <c r="B30" s="144" t="n">
         <v>15.0</v>
       </c>
-      <c r="C30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="G30" s="43" t="s">
-        <v>83</v>
+      <c r="C30" s="145"/>
+      <c r="E30" s="145"/>
+      <c r="G30" s="143" t="n">
+        <f>((E30-C30)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="31" ht="14.4" customHeight="true">
-      <c r="B31" s="43" t="n">
+      <c r="B31" s="144" t="n">
         <v>16.0</v>
       </c>
-      <c r="C31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="G31" s="43" t="s">
-        <v>83</v>
+      <c r="C31" s="145"/>
+      <c r="E31" s="145"/>
+      <c r="G31" s="143" t="n">
+        <f>((E31-C31)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="32" ht="14.4" customHeight="true">
-      <c r="B32" s="43" t="n">
+      <c r="B32" s="144" t="n">
         <v>17.0</v>
       </c>
-      <c r="C32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="G32" s="43" t="s">
-        <v>83</v>
+      <c r="C32" s="145"/>
+      <c r="E32" s="145"/>
+      <c r="G32" s="143" t="n">
+        <f>((E32-C32)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="33" ht="14.4" customHeight="true">
-      <c r="B33" s="43" t="n">
+      <c r="B33" s="144" t="n">
         <v>18.0</v>
       </c>
-      <c r="C33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="G33" s="43" t="s">
-        <v>83</v>
+      <c r="C33" s="145"/>
+      <c r="E33" s="145"/>
+      <c r="G33" s="143" t="n">
+        <f>((E33-C33)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="34" ht="14.4" customHeight="true">
-      <c r="B34" s="43" t="n">
+      <c r="B34" s="144" t="n">
         <v>19.0</v>
       </c>
-      <c r="C34" s="43"/>
-      <c r="E34" s="43"/>
-      <c r="G34" s="43" t="s">
-        <v>83</v>
+      <c r="C34" s="145"/>
+      <c r="E34" s="145"/>
+      <c r="G34" s="143" t="n">
+        <f>((E34-C34)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="35" ht="14.4" customHeight="true">
@@ -10982,53 +11100,58 @@
       </c>
     </row>
     <row r="37" ht="14.4" customHeight="true">
-      <c r="B37" s="46" t="n">
+      <c r="B37" s="144" t="n">
         <v>22.0</v>
       </c>
-      <c r="C37" s="46"/>
-      <c r="E37" s="46"/>
-      <c r="G37" s="46" t="s">
-        <v>83</v>
+      <c r="C37" s="145"/>
+      <c r="E37" s="145"/>
+      <c r="G37" s="143" t="n">
+        <f>((E37-C37)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="38" ht="14.4" customHeight="true">
-      <c r="B38" s="46" t="n">
+      <c r="B38" s="144" t="n">
         <v>23.0</v>
       </c>
-      <c r="C38" s="46"/>
-      <c r="E38" s="46"/>
-      <c r="G38" s="46" t="s">
-        <v>83</v>
+      <c r="C38" s="145"/>
+      <c r="E38" s="145"/>
+      <c r="G38" s="143" t="n">
+        <f>((E38-C38)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="39" ht="14.4" customHeight="true">
-      <c r="B39" s="46" t="n">
+      <c r="B39" s="144" t="n">
         <v>24.0</v>
       </c>
-      <c r="C39" s="46"/>
-      <c r="E39" s="46"/>
-      <c r="G39" s="46" t="s">
-        <v>83</v>
+      <c r="C39" s="145"/>
+      <c r="E39" s="145"/>
+      <c r="G39" s="143" t="n">
+        <f>((E39-C39)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="40" ht="14.4" customHeight="true">
-      <c r="B40" s="46" t="n">
+      <c r="B40" s="144" t="n">
         <v>25.0</v>
       </c>
-      <c r="C40" s="46"/>
-      <c r="E40" s="46"/>
-      <c r="G40" s="46" t="s">
-        <v>83</v>
+      <c r="C40" s="145"/>
+      <c r="E40" s="145"/>
+      <c r="G40" s="143" t="n">
+        <f>((E40-C40)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="41" ht="14.4" customHeight="true">
-      <c r="B41" s="46" t="n">
+      <c r="B41" s="144" t="n">
         <v>26.0</v>
       </c>
-      <c r="C41" s="46"/>
-      <c r="E41" s="46"/>
-      <c r="G41" s="46" t="s">
-        <v>83</v>
+      <c r="C41" s="145"/>
+      <c r="E41" s="145"/>
+      <c r="G41" s="143" t="n">
+        <f>((E41-C41)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="42" ht="14.4" customHeight="true">
@@ -11337,53 +11460,58 @@
       <c r="G15" s="175"/>
     </row>
     <row r="16" ht="14.4" customHeight="true">
-      <c r="B16" s="29" t="n">
+      <c r="B16" s="176" t="n">
         <v>1.0</v>
       </c>
-      <c r="C16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="G16" s="29" t="s">
-        <v>83</v>
+      <c r="C16" s="177"/>
+      <c r="E16" s="177"/>
+      <c r="G16" s="175" t="n">
+        <f>((E16-C16)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="17" ht="14.4" customHeight="true">
-      <c r="B17" s="30" t="n">
+      <c r="B17" s="176" t="n">
         <v>2.0</v>
       </c>
-      <c r="C17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="G17" s="30" t="s">
-        <v>83</v>
+      <c r="C17" s="177"/>
+      <c r="E17" s="177"/>
+      <c r="G17" s="175" t="n">
+        <f>((E17-C17)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="18" ht="14.4" customHeight="true">
-      <c r="B18" s="30" t="n">
+      <c r="B18" s="176" t="n">
         <v>3.0</v>
       </c>
-      <c r="C18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="G18" s="30" t="s">
-        <v>83</v>
+      <c r="C18" s="177"/>
+      <c r="E18" s="177"/>
+      <c r="G18" s="175" t="n">
+        <f>((E18-C18)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="19" ht="14.4" customHeight="true">
-      <c r="B19" s="30" t="n">
+      <c r="B19" s="176" t="n">
         <v>4.0</v>
       </c>
-      <c r="C19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="G19" s="30" t="s">
-        <v>83</v>
+      <c r="C19" s="177"/>
+      <c r="E19" s="177"/>
+      <c r="G19" s="175" t="n">
+        <f>((E19-C19)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="20" ht="14.4" customHeight="true">
-      <c r="B20" s="30" t="n">
+      <c r="B20" s="176" t="n">
         <v>5.0</v>
       </c>
-      <c r="C20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="G20" s="30" t="s">
-        <v>83</v>
+      <c r="C20" s="177"/>
+      <c r="E20" s="177"/>
+      <c r="G20" s="175" t="n">
+        <f>((E20-C20)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="21" ht="14.4" customHeight="true">
@@ -11407,53 +11535,58 @@
       </c>
     </row>
     <row r="23" ht="14.4" customHeight="true">
-      <c r="B23" s="36" t="n">
+      <c r="B23" s="176" t="n">
         <v>8.0</v>
       </c>
-      <c r="C23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="G23" s="36" t="s">
-        <v>83</v>
+      <c r="C23" s="177"/>
+      <c r="E23" s="177"/>
+      <c r="G23" s="175" t="n">
+        <f>((E23-C23)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="24" ht="14.4" customHeight="true">
-      <c r="B24" s="36" t="n">
+      <c r="B24" s="176" t="n">
         <v>9.0</v>
       </c>
-      <c r="C24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="G24" s="36" t="s">
-        <v>83</v>
+      <c r="C24" s="177"/>
+      <c r="E24" s="177"/>
+      <c r="G24" s="175" t="n">
+        <f>((E24-C24)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="25" ht="14.4" customHeight="true">
-      <c r="B25" s="36" t="n">
+      <c r="B25" s="176" t="n">
         <v>10.0</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="G25" s="36" t="s">
-        <v>83</v>
+      <c r="C25" s="177"/>
+      <c r="E25" s="177"/>
+      <c r="G25" s="175" t="n">
+        <f>((E25-C25)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="26" ht="14.4" customHeight="true">
-      <c r="B26" s="36" t="n">
+      <c r="B26" s="176" t="n">
         <v>11.0</v>
       </c>
-      <c r="C26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="G26" s="36" t="s">
-        <v>83</v>
+      <c r="C26" s="177"/>
+      <c r="E26" s="177"/>
+      <c r="G26" s="175" t="n">
+        <f>((E26-C26)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="27" ht="14.4" customHeight="true">
-      <c r="B27" s="36" t="n">
+      <c r="B27" s="176" t="n">
         <v>12.0</v>
       </c>
-      <c r="C27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="G27" s="36" t="s">
-        <v>83</v>
+      <c r="C27" s="177"/>
+      <c r="E27" s="177"/>
+      <c r="G27" s="175" t="n">
+        <f>((E27-C27)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="28" ht="14.4" customHeight="true">
@@ -11477,53 +11610,58 @@
       </c>
     </row>
     <row r="30" ht="14.4" customHeight="true">
-      <c r="B30" s="43" t="n">
+      <c r="B30" s="176" t="n">
         <v>15.0</v>
       </c>
-      <c r="C30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="G30" s="43" t="s">
-        <v>83</v>
+      <c r="C30" s="177"/>
+      <c r="E30" s="177"/>
+      <c r="G30" s="175" t="n">
+        <f>((E30-C30)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="31" ht="14.4" customHeight="true">
-      <c r="B31" s="43" t="n">
+      <c r="B31" s="176" t="n">
         <v>16.0</v>
       </c>
-      <c r="C31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="G31" s="43" t="s">
-        <v>83</v>
+      <c r="C31" s="177"/>
+      <c r="E31" s="177"/>
+      <c r="G31" s="175" t="n">
+        <f>((E31-C31)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="32" ht="14.4" customHeight="true">
-      <c r="B32" s="43" t="n">
+      <c r="B32" s="176" t="n">
         <v>17.0</v>
       </c>
-      <c r="C32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="G32" s="43" t="s">
-        <v>83</v>
+      <c r="C32" s="177"/>
+      <c r="E32" s="177"/>
+      <c r="G32" s="175" t="n">
+        <f>((E32-C32)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="33" ht="14.4" customHeight="true">
-      <c r="B33" s="43" t="n">
+      <c r="B33" s="176" t="n">
         <v>18.0</v>
       </c>
-      <c r="C33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="G33" s="43" t="s">
-        <v>83</v>
+      <c r="C33" s="177"/>
+      <c r="E33" s="177"/>
+      <c r="G33" s="175" t="n">
+        <f>((E33-C33)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="34" ht="14.4" customHeight="true">
-      <c r="B34" s="43" t="n">
+      <c r="B34" s="176" t="n">
         <v>19.0</v>
       </c>
-      <c r="C34" s="43"/>
-      <c r="E34" s="43"/>
-      <c r="G34" s="43" t="s">
-        <v>83</v>
+      <c r="C34" s="177"/>
+      <c r="E34" s="177"/>
+      <c r="G34" s="175" t="n">
+        <f>((E34-C34)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="35" ht="14.4" customHeight="true">
@@ -11547,53 +11685,58 @@
       </c>
     </row>
     <row r="37" ht="14.4" customHeight="true">
-      <c r="B37" s="46" t="n">
+      <c r="B37" s="176" t="n">
         <v>22.0</v>
       </c>
-      <c r="C37" s="46"/>
-      <c r="E37" s="46"/>
-      <c r="G37" s="46" t="s">
-        <v>83</v>
+      <c r="C37" s="177"/>
+      <c r="E37" s="177"/>
+      <c r="G37" s="175" t="n">
+        <f>((E37-C37)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="38" ht="14.4" customHeight="true">
-      <c r="B38" s="46" t="n">
+      <c r="B38" s="176" t="n">
         <v>23.0</v>
       </c>
-      <c r="C38" s="46"/>
-      <c r="E38" s="46"/>
-      <c r="G38" s="46" t="s">
-        <v>83</v>
+      <c r="C38" s="177"/>
+      <c r="E38" s="177"/>
+      <c r="G38" s="175" t="n">
+        <f>((E38-C38)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="39" ht="14.4" customHeight="true">
-      <c r="B39" s="46" t="n">
+      <c r="B39" s="176" t="n">
         <v>24.0</v>
       </c>
-      <c r="C39" s="46"/>
-      <c r="E39" s="46"/>
-      <c r="G39" s="46" t="s">
-        <v>83</v>
+      <c r="C39" s="177"/>
+      <c r="E39" s="177"/>
+      <c r="G39" s="175" t="n">
+        <f>((E39-C39)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="40" ht="14.4" customHeight="true">
-      <c r="B40" s="46" t="n">
+      <c r="B40" s="176" t="n">
         <v>25.0</v>
       </c>
-      <c r="C40" s="46"/>
-      <c r="E40" s="46"/>
-      <c r="G40" s="46" t="s">
-        <v>83</v>
+      <c r="C40" s="177"/>
+      <c r="E40" s="177"/>
+      <c r="G40" s="175" t="n">
+        <f>((E40-C40)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="41" ht="14.4" customHeight="true">
-      <c r="B41" s="46" t="n">
+      <c r="B41" s="176" t="n">
         <v>26.0</v>
       </c>
-      <c r="C41" s="46"/>
-      <c r="E41" s="46"/>
-      <c r="G41" s="46" t="s">
-        <v>83</v>
+      <c r="C41" s="177"/>
+      <c r="E41" s="177"/>
+      <c r="G41" s="175" t="n">
+        <f>((E41-C41)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="42" ht="14.4" customHeight="true">
@@ -11617,33 +11760,36 @@
       </c>
     </row>
     <row r="44" ht="14.4" customHeight="true">
-      <c r="B44" s="56" t="n">
+      <c r="B44" s="176" t="n">
         <v>29.0</v>
       </c>
-      <c r="C44" s="56"/>
-      <c r="E44" s="56"/>
-      <c r="G44" s="56" t="s">
-        <v>83</v>
+      <c r="C44" s="177"/>
+      <c r="E44" s="177"/>
+      <c r="G44" s="175" t="n">
+        <f>((E44-C44)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="45" ht="14.4" customHeight="true">
-      <c r="B45" s="56" t="n">
+      <c r="B45" s="176" t="n">
         <v>30.0</v>
       </c>
-      <c r="C45" s="56"/>
-      <c r="E45" s="56"/>
-      <c r="G45" s="56" t="s">
-        <v>83</v>
+      <c r="C45" s="177"/>
+      <c r="E45" s="177"/>
+      <c r="G45" s="175" t="n">
+        <f>((E45-C45)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="46" ht="14.4" customHeight="true">
-      <c r="B46" s="57" t="n">
+      <c r="B46" s="176" t="n">
         <v>31.0</v>
       </c>
-      <c r="C46" s="57"/>
-      <c r="E46" s="57"/>
-      <c r="G46" s="57" t="s">
-        <v>83</v>
+      <c r="C46" s="177"/>
+      <c r="E46" s="177"/>
+      <c r="G46" s="175" t="n">
+        <f>((E46-C46)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="47" ht="14.4" customHeight="true">
@@ -11912,13 +12058,14 @@
       <c r="G15" s="206"/>
     </row>
     <row r="16" ht="14.4" customHeight="true">
-      <c r="B16" s="29" t="n">
+      <c r="B16" s="207" t="n">
         <v>1.0</v>
       </c>
-      <c r="C16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="G16" s="29" t="s">
-        <v>83</v>
+      <c r="C16" s="208"/>
+      <c r="E16" s="208"/>
+      <c r="G16" s="206" t="n">
+        <f>((E16-C16)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="17" ht="14.4" customHeight="true">
@@ -11962,43 +12109,47 @@
       </c>
     </row>
     <row r="21" ht="14.4" customHeight="true">
-      <c r="B21" s="36" t="n">
+      <c r="B21" s="207" t="n">
         <v>6.0</v>
       </c>
-      <c r="C21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="G21" s="36" t="s">
-        <v>83</v>
+      <c r="C21" s="208"/>
+      <c r="E21" s="208"/>
+      <c r="G21" s="206" t="n">
+        <f>((E21-C21)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="22" ht="14.4" customHeight="true">
-      <c r="B22" s="36" t="n">
+      <c r="B22" s="207" t="n">
         <v>7.0</v>
       </c>
-      <c r="C22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="G22" s="36" t="s">
-        <v>83</v>
+      <c r="C22" s="208"/>
+      <c r="E22" s="208"/>
+      <c r="G22" s="206" t="n">
+        <f>((E22-C22)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="23" ht="14.4" customHeight="true">
-      <c r="B23" s="36" t="n">
+      <c r="B23" s="207" t="n">
         <v>8.0</v>
       </c>
-      <c r="C23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="G23" s="36" t="s">
-        <v>83</v>
+      <c r="C23" s="208"/>
+      <c r="E23" s="208"/>
+      <c r="G23" s="206" t="n">
+        <f>((E23-C23)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="24" ht="14.4" customHeight="true">
-      <c r="B24" s="36" t="n">
+      <c r="B24" s="207" t="n">
         <v>9.0</v>
       </c>
-      <c r="C24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="G24" s="36" t="s">
-        <v>83</v>
+      <c r="C24" s="208"/>
+      <c r="E24" s="208"/>
+      <c r="G24" s="206" t="n">
+        <f>((E24-C24)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="25" ht="14.4" customHeight="true">
@@ -12022,53 +12173,58 @@
       </c>
     </row>
     <row r="27" ht="14.4" customHeight="true">
-      <c r="B27" s="43" t="n">
+      <c r="B27" s="207" t="n">
         <v>12.0</v>
       </c>
-      <c r="C27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="G27" s="43" t="s">
-        <v>83</v>
+      <c r="C27" s="208"/>
+      <c r="E27" s="208"/>
+      <c r="G27" s="206" t="n">
+        <f>((E27-C27)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="28" ht="14.4" customHeight="true">
-      <c r="B28" s="43" t="n">
+      <c r="B28" s="207" t="n">
         <v>13.0</v>
       </c>
-      <c r="C28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="G28" s="43" t="s">
-        <v>83</v>
+      <c r="C28" s="208"/>
+      <c r="E28" s="208"/>
+      <c r="G28" s="206" t="n">
+        <f>((E28-C28)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="29" ht="14.4" customHeight="true">
-      <c r="B29" s="43" t="n">
+      <c r="B29" s="207" t="n">
         <v>14.0</v>
       </c>
-      <c r="C29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="G29" s="43" t="s">
-        <v>83</v>
+      <c r="C29" s="208"/>
+      <c r="E29" s="208"/>
+      <c r="G29" s="206" t="n">
+        <f>((E29-C29)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="30" ht="14.4" customHeight="true">
-      <c r="B30" s="43" t="n">
+      <c r="B30" s="207" t="n">
         <v>15.0</v>
       </c>
-      <c r="C30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="G30" s="43" t="s">
-        <v>83</v>
+      <c r="C30" s="208"/>
+      <c r="E30" s="208"/>
+      <c r="G30" s="206" t="n">
+        <f>((E30-C30)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="31" ht="14.4" customHeight="true">
-      <c r="B31" s="43" t="n">
+      <c r="B31" s="207" t="n">
         <v>16.0</v>
       </c>
-      <c r="C31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="G31" s="43" t="s">
-        <v>83</v>
+      <c r="C31" s="208"/>
+      <c r="E31" s="208"/>
+      <c r="G31" s="206" t="n">
+        <f>((E31-C31)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="32" ht="14.4" customHeight="true">
@@ -12092,53 +12248,58 @@
       </c>
     </row>
     <row r="34" ht="14.4" customHeight="true">
-      <c r="B34" s="46" t="n">
+      <c r="B34" s="207" t="n">
         <v>19.0</v>
       </c>
-      <c r="C34" s="46"/>
-      <c r="E34" s="46"/>
-      <c r="G34" s="46" t="s">
-        <v>83</v>
+      <c r="C34" s="208"/>
+      <c r="E34" s="208"/>
+      <c r="G34" s="206" t="n">
+        <f>((E34-C34)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="35" ht="14.4" customHeight="true">
-      <c r="B35" s="46" t="n">
+      <c r="B35" s="207" t="n">
         <v>20.0</v>
       </c>
-      <c r="C35" s="46"/>
-      <c r="E35" s="46"/>
-      <c r="G35" s="46" t="s">
-        <v>83</v>
+      <c r="C35" s="208"/>
+      <c r="E35" s="208"/>
+      <c r="G35" s="206" t="n">
+        <f>((E35-C35)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="36" ht="14.4" customHeight="true">
-      <c r="B36" s="46" t="n">
+      <c r="B36" s="207" t="n">
         <v>21.0</v>
       </c>
-      <c r="C36" s="46"/>
-      <c r="E36" s="46"/>
-      <c r="G36" s="46" t="s">
-        <v>83</v>
+      <c r="C36" s="208"/>
+      <c r="E36" s="208"/>
+      <c r="G36" s="206" t="n">
+        <f>((E36-C36)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="37" ht="14.4" customHeight="true">
-      <c r="B37" s="46" t="n">
+      <c r="B37" s="207" t="n">
         <v>22.0</v>
       </c>
-      <c r="C37" s="46"/>
-      <c r="E37" s="46"/>
-      <c r="G37" s="46" t="s">
-        <v>83</v>
+      <c r="C37" s="208"/>
+      <c r="E37" s="208"/>
+      <c r="G37" s="206" t="n">
+        <f>((E37-C37)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="38" ht="14.4" customHeight="true">
-      <c r="B38" s="46" t="n">
+      <c r="B38" s="207" t="n">
         <v>23.0</v>
       </c>
-      <c r="C38" s="46"/>
-      <c r="E38" s="46"/>
-      <c r="G38" s="46" t="s">
-        <v>83</v>
+      <c r="C38" s="208"/>
+      <c r="E38" s="208"/>
+      <c r="G38" s="206" t="n">
+        <f>((E38-C38)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="39" ht="14.4" customHeight="true">
@@ -12162,53 +12323,58 @@
       </c>
     </row>
     <row r="41" ht="14.4" customHeight="true">
-      <c r="B41" s="56" t="n">
+      <c r="B41" s="207" t="n">
         <v>26.0</v>
       </c>
-      <c r="C41" s="56"/>
-      <c r="E41" s="56"/>
-      <c r="G41" s="56" t="s">
-        <v>83</v>
+      <c r="C41" s="208"/>
+      <c r="E41" s="208"/>
+      <c r="G41" s="206" t="n">
+        <f>((E41-C41)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="42" ht="14.4" customHeight="true">
-      <c r="B42" s="56" t="n">
+      <c r="B42" s="207" t="n">
         <v>27.0</v>
       </c>
-      <c r="C42" s="56"/>
-      <c r="E42" s="56"/>
-      <c r="G42" s="56" t="s">
-        <v>83</v>
+      <c r="C42" s="208"/>
+      <c r="E42" s="208"/>
+      <c r="G42" s="206" t="n">
+        <f>((E42-C42)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="43" ht="14.4" customHeight="true">
-      <c r="B43" s="56" t="n">
+      <c r="B43" s="207" t="n">
         <v>28.0</v>
       </c>
-      <c r="C43" s="56"/>
-      <c r="E43" s="56"/>
-      <c r="G43" s="56" t="s">
-        <v>83</v>
+      <c r="C43" s="208"/>
+      <c r="E43" s="208"/>
+      <c r="G43" s="206" t="n">
+        <f>((E43-C43)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="44" ht="14.4" customHeight="true">
-      <c r="B44" s="56" t="n">
+      <c r="B44" s="207" t="n">
         <v>29.0</v>
       </c>
-      <c r="C44" s="56"/>
-      <c r="E44" s="56"/>
-      <c r="G44" s="56" t="s">
-        <v>83</v>
+      <c r="C44" s="208"/>
+      <c r="E44" s="208"/>
+      <c r="G44" s="206" t="n">
+        <f>((E44-C44)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="45" ht="14.4" customHeight="true">
-      <c r="B45" s="57" t="n">
+      <c r="B45" s="207" t="n">
         <v>30.0</v>
       </c>
-      <c r="C45" s="57"/>
-      <c r="E45" s="57"/>
-      <c r="G45" s="57" t="s">
-        <v>83</v>
+      <c r="C45" s="208"/>
+      <c r="E45" s="208"/>
+      <c r="G45" s="206" t="n">
+        <f>((E45-C45)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="46" ht="14.4" customHeight="true">
@@ -12502,53 +12668,58 @@
       </c>
     </row>
     <row r="18" ht="14.4" customHeight="true">
-      <c r="B18" s="36" t="n">
+      <c r="B18" s="238" t="n">
         <v>3.0</v>
       </c>
-      <c r="C18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="G18" s="36" t="s">
-        <v>83</v>
+      <c r="C18" s="239"/>
+      <c r="E18" s="239"/>
+      <c r="G18" s="237" t="n">
+        <f>((E18-C18)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="19" ht="14.4" customHeight="true">
-      <c r="B19" s="36" t="n">
+      <c r="B19" s="238" t="n">
         <v>4.0</v>
       </c>
-      <c r="C19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="G19" s="36" t="s">
-        <v>83</v>
+      <c r="C19" s="239"/>
+      <c r="E19" s="239"/>
+      <c r="G19" s="237" t="n">
+        <f>((E19-C19)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="20" ht="14.4" customHeight="true">
-      <c r="B20" s="36" t="n">
+      <c r="B20" s="238" t="n">
         <v>5.0</v>
       </c>
-      <c r="C20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="G20" s="36" t="s">
-        <v>83</v>
+      <c r="C20" s="239"/>
+      <c r="E20" s="239"/>
+      <c r="G20" s="237" t="n">
+        <f>((E20-C20)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="21" ht="14.4" customHeight="true">
-      <c r="B21" s="36" t="n">
+      <c r="B21" s="238" t="n">
         <v>6.0</v>
       </c>
-      <c r="C21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="G21" s="36" t="s">
-        <v>83</v>
+      <c r="C21" s="239"/>
+      <c r="E21" s="239"/>
+      <c r="G21" s="237" t="n">
+        <f>((E21-C21)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="22" ht="14.4" customHeight="true">
-      <c r="B22" s="36" t="n">
+      <c r="B22" s="238" t="n">
         <v>7.0</v>
       </c>
-      <c r="C22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="G22" s="36" t="s">
-        <v>83</v>
+      <c r="C22" s="239"/>
+      <c r="E22" s="239"/>
+      <c r="G22" s="237" t="n">
+        <f>((E22-C22)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="23" ht="14.4" customHeight="true">
@@ -12572,53 +12743,58 @@
       </c>
     </row>
     <row r="25" ht="14.4" customHeight="true">
-      <c r="B25" s="43" t="n">
+      <c r="B25" s="238" t="n">
         <v>10.0</v>
       </c>
-      <c r="C25" s="43"/>
-      <c r="E25" s="43"/>
-      <c r="G25" s="43" t="s">
-        <v>83</v>
+      <c r="C25" s="239"/>
+      <c r="E25" s="239"/>
+      <c r="G25" s="237" t="n">
+        <f>((E25-C25)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="26" ht="14.4" customHeight="true">
-      <c r="B26" s="43" t="n">
+      <c r="B26" s="238" t="n">
         <v>11.0</v>
       </c>
-      <c r="C26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="G26" s="43" t="s">
-        <v>83</v>
+      <c r="C26" s="239"/>
+      <c r="E26" s="239"/>
+      <c r="G26" s="237" t="n">
+        <f>((E26-C26)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="27" ht="14.4" customHeight="true">
-      <c r="B27" s="43" t="n">
+      <c r="B27" s="238" t="n">
         <v>12.0</v>
       </c>
-      <c r="C27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="G27" s="43" t="s">
-        <v>83</v>
+      <c r="C27" s="239"/>
+      <c r="E27" s="239"/>
+      <c r="G27" s="237" t="n">
+        <f>((E27-C27)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="28" ht="14.4" customHeight="true">
-      <c r="B28" s="43" t="n">
+      <c r="B28" s="238" t="n">
         <v>13.0</v>
       </c>
-      <c r="C28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="G28" s="43" t="s">
-        <v>83</v>
+      <c r="C28" s="239"/>
+      <c r="E28" s="239"/>
+      <c r="G28" s="237" t="n">
+        <f>((E28-C28)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="29" ht="14.4" customHeight="true">
-      <c r="B29" s="43" t="n">
+      <c r="B29" s="238" t="n">
         <v>14.0</v>
       </c>
-      <c r="C29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="G29" s="43" t="s">
-        <v>83</v>
+      <c r="C29" s="239"/>
+      <c r="E29" s="239"/>
+      <c r="G29" s="237" t="n">
+        <f>((E29-C29)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="30" ht="14.4" customHeight="true">
@@ -12642,53 +12818,58 @@
       </c>
     </row>
     <row r="32" ht="14.4" customHeight="true">
-      <c r="B32" s="43" t="n">
+      <c r="B32" s="238" t="n">
         <v>17.0</v>
       </c>
-      <c r="C32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="G32" s="43" t="s">
-        <v>83</v>
+      <c r="C32" s="239"/>
+      <c r="E32" s="239"/>
+      <c r="G32" s="237" t="n">
+        <f>((E32-C32)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="33" ht="14.4" customHeight="true">
-      <c r="B33" s="43" t="n">
+      <c r="B33" s="238" t="n">
         <v>18.0</v>
       </c>
-      <c r="C33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="G33" s="43" t="s">
-        <v>83</v>
+      <c r="C33" s="239"/>
+      <c r="E33" s="239"/>
+      <c r="G33" s="237" t="n">
+        <f>((E33-C33)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="34" ht="14.4" customHeight="true">
-      <c r="B34" s="43" t="n">
+      <c r="B34" s="238" t="n">
         <v>19.0</v>
       </c>
-      <c r="C34" s="43"/>
-      <c r="E34" s="43"/>
-      <c r="G34" s="43" t="s">
-        <v>83</v>
+      <c r="C34" s="239"/>
+      <c r="E34" s="239"/>
+      <c r="G34" s="237" t="n">
+        <f>((E34-C34)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="35" ht="14.4" customHeight="true">
-      <c r="B35" s="43" t="n">
+      <c r="B35" s="238" t="n">
         <v>20.0</v>
       </c>
-      <c r="C35" s="43"/>
-      <c r="E35" s="43"/>
-      <c r="G35" s="43" t="s">
-        <v>83</v>
+      <c r="C35" s="239"/>
+      <c r="E35" s="239"/>
+      <c r="G35" s="237" t="n">
+        <f>((E35-C35)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="36" ht="14.4" customHeight="true">
-      <c r="B36" s="43" t="n">
+      <c r="B36" s="238" t="n">
         <v>21.0</v>
       </c>
-      <c r="C36" s="43"/>
-      <c r="E36" s="43"/>
-      <c r="G36" s="43" t="s">
-        <v>83</v>
+      <c r="C36" s="239"/>
+      <c r="E36" s="239"/>
+      <c r="G36" s="237" t="n">
+        <f>((E36-C36)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="37" ht="14.4" customHeight="true">
@@ -12712,53 +12893,58 @@
       </c>
     </row>
     <row r="39" ht="14.4" customHeight="true">
-      <c r="B39" s="46" t="n">
+      <c r="B39" s="238" t="n">
         <v>24.0</v>
       </c>
-      <c r="C39" s="46"/>
-      <c r="E39" s="46"/>
-      <c r="G39" s="46" t="s">
-        <v>83</v>
+      <c r="C39" s="239"/>
+      <c r="E39" s="239"/>
+      <c r="G39" s="237" t="n">
+        <f>((E39-C39)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="40" ht="14.4" customHeight="true">
-      <c r="B40" s="46" t="n">
+      <c r="B40" s="238" t="n">
         <v>25.0</v>
       </c>
-      <c r="C40" s="46"/>
-      <c r="E40" s="46"/>
-      <c r="G40" s="46" t="s">
-        <v>83</v>
+      <c r="C40" s="239"/>
+      <c r="E40" s="239"/>
+      <c r="G40" s="237" t="n">
+        <f>((E40-C40)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="41" ht="14.4" customHeight="true">
-      <c r="B41" s="46" t="n">
+      <c r="B41" s="238" t="n">
         <v>26.0</v>
       </c>
-      <c r="C41" s="46"/>
-      <c r="E41" s="46"/>
-      <c r="G41" s="46" t="s">
-        <v>83</v>
+      <c r="C41" s="239"/>
+      <c r="E41" s="239"/>
+      <c r="G41" s="237" t="n">
+        <f>((E41-C41)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="42" ht="14.4" customHeight="true">
-      <c r="B42" s="46" t="n">
+      <c r="B42" s="238" t="n">
         <v>27.0</v>
       </c>
-      <c r="C42" s="46"/>
-      <c r="E42" s="46"/>
-      <c r="G42" s="46" t="s">
-        <v>83</v>
+      <c r="C42" s="239"/>
+      <c r="E42" s="239"/>
+      <c r="G42" s="237" t="n">
+        <f>((E42-C42)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="43" ht="14.4" customHeight="true">
-      <c r="B43" s="46" t="n">
+      <c r="B43" s="238" t="n">
         <v>28.0</v>
       </c>
-      <c r="C43" s="46"/>
-      <c r="E43" s="46"/>
-      <c r="G43" s="46" t="s">
-        <v>83</v>
+      <c r="C43" s="239"/>
+      <c r="E43" s="239"/>
+      <c r="G43" s="237" t="n">
+        <f>((E43-C43)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="44" ht="14.4" customHeight="true">
@@ -12782,13 +12968,14 @@
       </c>
     </row>
     <row r="46" ht="14.4" customHeight="true">
-      <c r="B46" s="57" t="n">
+      <c r="B46" s="238" t="n">
         <v>31.0</v>
       </c>
-      <c r="C46" s="57"/>
-      <c r="E46" s="57"/>
-      <c r="G46" s="57" t="s">
-        <v>83</v>
+      <c r="C46" s="239"/>
+      <c r="E46" s="239"/>
+      <c r="G46" s="237" t="n">
+        <f>((E46-C46)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="47" ht="14.4" customHeight="true">
@@ -13056,33 +13243,36 @@
       </c>
     </row>
     <row r="17" ht="14.4" customHeight="true">
-      <c r="B17" s="30" t="n">
+      <c r="B17" s="268" t="n">
         <v>2.0</v>
       </c>
-      <c r="C17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="G17" s="30" t="s">
-        <v>83</v>
+      <c r="C17" s="269"/>
+      <c r="E17" s="269"/>
+      <c r="G17" s="267" t="n">
+        <f>((E17-C17)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="18" ht="14.4" customHeight="true">
-      <c r="B18" s="30" t="n">
+      <c r="B18" s="268" t="n">
         <v>3.0</v>
       </c>
-      <c r="C18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="G18" s="30" t="s">
-        <v>83</v>
+      <c r="C18" s="269"/>
+      <c r="E18" s="269"/>
+      <c r="G18" s="267" t="n">
+        <f>((E18-C18)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="19" ht="14.4" customHeight="true">
-      <c r="B19" s="30" t="n">
+      <c r="B19" s="268" t="n">
         <v>4.0</v>
       </c>
-      <c r="C19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="G19" s="30" t="s">
-        <v>83</v>
+      <c r="C19" s="269"/>
+      <c r="E19" s="269"/>
+      <c r="G19" s="267" t="n">
+        <f>((E19-C19)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="20" ht="14.4" customHeight="true">
@@ -13106,53 +13296,58 @@
       </c>
     </row>
     <row r="22" ht="14.4" customHeight="true">
-      <c r="B22" s="36" t="n">
+      <c r="B22" s="268" t="n">
         <v>7.0</v>
       </c>
-      <c r="C22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="G22" s="36" t="s">
-        <v>83</v>
+      <c r="C22" s="269"/>
+      <c r="E22" s="269"/>
+      <c r="G22" s="267" t="n">
+        <f>((E22-C22)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="23" ht="14.4" customHeight="true">
-      <c r="B23" s="36" t="n">
+      <c r="B23" s="268" t="n">
         <v>8.0</v>
       </c>
-      <c r="C23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="G23" s="36" t="s">
-        <v>83</v>
+      <c r="C23" s="269"/>
+      <c r="E23" s="269"/>
+      <c r="G23" s="267" t="n">
+        <f>((E23-C23)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="24" ht="14.4" customHeight="true">
-      <c r="B24" s="36" t="n">
+      <c r="B24" s="268" t="n">
         <v>9.0</v>
       </c>
-      <c r="C24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="G24" s="36" t="s">
-        <v>83</v>
+      <c r="C24" s="269"/>
+      <c r="E24" s="269"/>
+      <c r="G24" s="267" t="n">
+        <f>((E24-C24)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="25" ht="14.4" customHeight="true">
-      <c r="B25" s="36" t="n">
+      <c r="B25" s="268" t="n">
         <v>10.0</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="G25" s="36" t="s">
-        <v>83</v>
+      <c r="C25" s="269"/>
+      <c r="E25" s="269"/>
+      <c r="G25" s="267" t="n">
+        <f>((E25-C25)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="26" ht="14.4" customHeight="true">
-      <c r="B26" s="36" t="n">
+      <c r="B26" s="268" t="n">
         <v>11.0</v>
       </c>
-      <c r="C26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="G26" s="36" t="s">
-        <v>83</v>
+      <c r="C26" s="269"/>
+      <c r="E26" s="269"/>
+      <c r="G26" s="267" t="n">
+        <f>((E26-C26)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="27" ht="14.4" customHeight="true">
@@ -13176,53 +13371,58 @@
       </c>
     </row>
     <row r="29" ht="14.4" customHeight="true">
-      <c r="B29" s="43" t="n">
+      <c r="B29" s="268" t="n">
         <v>14.0</v>
       </c>
-      <c r="C29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="G29" s="43" t="s">
-        <v>83</v>
+      <c r="C29" s="269"/>
+      <c r="E29" s="269"/>
+      <c r="G29" s="267" t="n">
+        <f>((E29-C29)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="30" ht="14.4" customHeight="true">
-      <c r="B30" s="43" t="n">
+      <c r="B30" s="268" t="n">
         <v>15.0</v>
       </c>
-      <c r="C30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="G30" s="43" t="s">
-        <v>83</v>
+      <c r="C30" s="269"/>
+      <c r="E30" s="269"/>
+      <c r="G30" s="267" t="n">
+        <f>((E30-C30)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="31" ht="14.4" customHeight="true">
-      <c r="B31" s="43" t="n">
+      <c r="B31" s="268" t="n">
         <v>16.0</v>
       </c>
-      <c r="C31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="G31" s="43" t="s">
-        <v>83</v>
+      <c r="C31" s="269"/>
+      <c r="E31" s="269"/>
+      <c r="G31" s="267" t="n">
+        <f>((E31-C31)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="32" ht="14.4" customHeight="true">
-      <c r="B32" s="43" t="n">
+      <c r="B32" s="268" t="n">
         <v>17.0</v>
       </c>
-      <c r="C32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="G32" s="43" t="s">
-        <v>83</v>
+      <c r="C32" s="269"/>
+      <c r="E32" s="269"/>
+      <c r="G32" s="267" t="n">
+        <f>((E32-C32)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="33" ht="14.4" customHeight="true">
-      <c r="B33" s="43" t="n">
+      <c r="B33" s="268" t="n">
         <v>18.0</v>
       </c>
-      <c r="C33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="G33" s="43" t="s">
-        <v>83</v>
+      <c r="C33" s="269"/>
+      <c r="E33" s="269"/>
+      <c r="G33" s="267" t="n">
+        <f>((E33-C33)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="34" ht="14.4" customHeight="true">
@@ -13246,33 +13446,36 @@
       </c>
     </row>
     <row r="36" ht="14.4" customHeight="true">
-      <c r="B36" s="46" t="n">
+      <c r="B36" s="268" t="n">
         <v>21.0</v>
       </c>
-      <c r="C36" s="46"/>
-      <c r="E36" s="46"/>
-      <c r="G36" s="46" t="s">
-        <v>83</v>
+      <c r="C36" s="269"/>
+      <c r="E36" s="269"/>
+      <c r="G36" s="267" t="n">
+        <f>((E36-C36)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="37" ht="14.4" customHeight="true">
-      <c r="B37" s="46" t="n">
+      <c r="B37" s="268" t="n">
         <v>22.0</v>
       </c>
-      <c r="C37" s="46"/>
-      <c r="E37" s="46"/>
-      <c r="G37" s="46" t="s">
-        <v>83</v>
+      <c r="C37" s="269"/>
+      <c r="E37" s="269"/>
+      <c r="G37" s="267" t="n">
+        <f>((E37-C37)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="38" ht="14.4" customHeight="true">
-      <c r="B38" s="46" t="n">
+      <c r="B38" s="268" t="n">
         <v>23.0</v>
       </c>
-      <c r="C38" s="46"/>
-      <c r="E38" s="46"/>
-      <c r="G38" s="46" t="s">
-        <v>83</v>
+      <c r="C38" s="269"/>
+      <c r="E38" s="269"/>
+      <c r="G38" s="267" t="n">
+        <f>((E38-C38)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="39" ht="14.4" customHeight="true">
@@ -13286,13 +13489,14 @@
       </c>
     </row>
     <row r="40" ht="14.4" customHeight="true">
-      <c r="B40" s="46" t="n">
+      <c r="B40" s="268" t="n">
         <v>25.0</v>
       </c>
-      <c r="C40" s="46"/>
-      <c r="E40" s="46"/>
-      <c r="G40" s="46" t="s">
-        <v>83</v>
+      <c r="C40" s="269"/>
+      <c r="E40" s="269"/>
+      <c r="G40" s="267" t="n">
+        <f>((E40-C40)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="41" ht="14.4" customHeight="true">
@@ -13316,33 +13520,36 @@
       </c>
     </row>
     <row r="43" ht="14.4" customHeight="true">
-      <c r="B43" s="56" t="n">
+      <c r="B43" s="268" t="n">
         <v>28.0</v>
       </c>
-      <c r="C43" s="56"/>
-      <c r="E43" s="56"/>
-      <c r="G43" s="56" t="s">
-        <v>83</v>
+      <c r="C43" s="269"/>
+      <c r="E43" s="269"/>
+      <c r="G43" s="267" t="n">
+        <f>((E43-C43)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="44" ht="14.4" customHeight="true">
-      <c r="B44" s="56" t="n">
+      <c r="B44" s="268" t="n">
         <v>29.0</v>
       </c>
-      <c r="C44" s="56"/>
-      <c r="E44" s="56"/>
-      <c r="G44" s="56" t="s">
-        <v>83</v>
+      <c r="C44" s="269"/>
+      <c r="E44" s="269"/>
+      <c r="G44" s="267" t="n">
+        <f>((E44-C44)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="45" ht="14.4" customHeight="true">
-      <c r="B45" s="57" t="n">
+      <c r="B45" s="268" t="n">
         <v>30.0</v>
       </c>
-      <c r="C45" s="57"/>
-      <c r="E45" s="57"/>
-      <c r="G45" s="57" t="s">
-        <v>83</v>
+      <c r="C45" s="269"/>
+      <c r="E45" s="269"/>
+      <c r="G45" s="267" t="n">
+        <f>((E45-C45)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="46"/>
@@ -13597,23 +13804,25 @@
       <c r="G15" s="295"/>
     </row>
     <row r="16" ht="14.4" customHeight="true">
-      <c r="B16" s="29" t="n">
+      <c r="B16" s="296" t="n">
         <v>1.0</v>
       </c>
-      <c r="C16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="G16" s="29" t="s">
-        <v>83</v>
+      <c r="C16" s="297"/>
+      <c r="E16" s="297"/>
+      <c r="G16" s="295" t="n">
+        <f>((E16-C16)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="17" ht="14.4" customHeight="true">
-      <c r="B17" s="30" t="n">
+      <c r="B17" s="296" t="n">
         <v>2.0</v>
       </c>
-      <c r="C17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="G17" s="30" t="s">
-        <v>83</v>
+      <c r="C17" s="297"/>
+      <c r="E17" s="297"/>
+      <c r="G17" s="295" t="n">
+        <f>((E17-C17)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="18" ht="14.4" customHeight="true">
@@ -13637,53 +13846,58 @@
       </c>
     </row>
     <row r="20" ht="14.4" customHeight="true">
-      <c r="B20" s="36" t="n">
+      <c r="B20" s="296" t="n">
         <v>5.0</v>
       </c>
-      <c r="C20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="G20" s="36" t="s">
-        <v>83</v>
+      <c r="C20" s="297"/>
+      <c r="E20" s="297"/>
+      <c r="G20" s="295" t="n">
+        <f>((E20-C20)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="21" ht="14.4" customHeight="true">
-      <c r="B21" s="36" t="n">
+      <c r="B21" s="296" t="n">
         <v>6.0</v>
       </c>
-      <c r="C21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="G21" s="36" t="s">
-        <v>83</v>
+      <c r="C21" s="297"/>
+      <c r="E21" s="297"/>
+      <c r="G21" s="295" t="n">
+        <f>((E21-C21)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="22" ht="14.4" customHeight="true">
-      <c r="B22" s="36" t="n">
+      <c r="B22" s="296" t="n">
         <v>7.0</v>
       </c>
-      <c r="C22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="G22" s="36" t="s">
-        <v>83</v>
+      <c r="C22" s="297"/>
+      <c r="E22" s="297"/>
+      <c r="G22" s="295" t="n">
+        <f>((E22-C22)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="23" ht="14.4" customHeight="true">
-      <c r="B23" s="36" t="n">
+      <c r="B23" s="296" t="n">
         <v>8.0</v>
       </c>
-      <c r="C23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="G23" s="36" t="s">
-        <v>83</v>
+      <c r="C23" s="297"/>
+      <c r="E23" s="297"/>
+      <c r="G23" s="295" t="n">
+        <f>((E23-C23)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="24" ht="14.4" customHeight="true">
-      <c r="B24" s="36" t="n">
+      <c r="B24" s="296" t="n">
         <v>9.0</v>
       </c>
-      <c r="C24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="G24" s="36" t="s">
-        <v>83</v>
+      <c r="C24" s="297"/>
+      <c r="E24" s="297"/>
+      <c r="G24" s="295" t="n">
+        <f>((E24-C24)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="25" ht="14.4" customHeight="true">
@@ -13707,53 +13921,58 @@
       </c>
     </row>
     <row r="27" ht="14.4" customHeight="true">
-      <c r="B27" s="43" t="n">
+      <c r="B27" s="296" t="n">
         <v>12.0</v>
       </c>
-      <c r="C27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="G27" s="43" t="s">
-        <v>83</v>
+      <c r="C27" s="297"/>
+      <c r="E27" s="297"/>
+      <c r="G27" s="295" t="n">
+        <f>((E27-C27)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="28" ht="14.4" customHeight="true">
-      <c r="B28" s="43" t="n">
+      <c r="B28" s="296" t="n">
         <v>13.0</v>
       </c>
-      <c r="C28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="G28" s="43" t="s">
-        <v>83</v>
+      <c r="C28" s="297"/>
+      <c r="E28" s="297"/>
+      <c r="G28" s="295" t="n">
+        <f>((E28-C28)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="29" ht="14.4" customHeight="true">
-      <c r="B29" s="43" t="n">
+      <c r="B29" s="296" t="n">
         <v>14.0</v>
       </c>
-      <c r="C29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="G29" s="43" t="s">
-        <v>83</v>
+      <c r="C29" s="297"/>
+      <c r="E29" s="297"/>
+      <c r="G29" s="295" t="n">
+        <f>((E29-C29)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="30" ht="14.4" customHeight="true">
-      <c r="B30" s="43" t="n">
+      <c r="B30" s="296" t="n">
         <v>15.0</v>
       </c>
-      <c r="C30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="G30" s="43" t="s">
-        <v>83</v>
+      <c r="C30" s="297"/>
+      <c r="E30" s="297"/>
+      <c r="G30" s="295" t="n">
+        <f>((E30-C30)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="31" ht="14.4" customHeight="true">
-      <c r="B31" s="43" t="n">
+      <c r="B31" s="296" t="n">
         <v>16.0</v>
       </c>
-      <c r="C31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="G31" s="43" t="s">
-        <v>83</v>
+      <c r="C31" s="297"/>
+      <c r="E31" s="297"/>
+      <c r="G31" s="295" t="n">
+        <f>((E31-C31)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="32" ht="14.4" customHeight="true">
@@ -13777,53 +13996,58 @@
       </c>
     </row>
     <row r="34" ht="14.4" customHeight="true">
-      <c r="B34" s="46" t="n">
+      <c r="B34" s="296" t="n">
         <v>19.0</v>
       </c>
-      <c r="C34" s="46"/>
-      <c r="E34" s="46"/>
-      <c r="G34" s="46" t="s">
-        <v>83</v>
+      <c r="C34" s="297"/>
+      <c r="E34" s="297"/>
+      <c r="G34" s="295" t="n">
+        <f>((E34-C34)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="35" ht="14.4" customHeight="true">
-      <c r="B35" s="46" t="n">
+      <c r="B35" s="296" t="n">
         <v>20.0</v>
       </c>
-      <c r="C35" s="46"/>
-      <c r="E35" s="46"/>
-      <c r="G35" s="46" t="s">
-        <v>83</v>
+      <c r="C35" s="297"/>
+      <c r="E35" s="297"/>
+      <c r="G35" s="295" t="n">
+        <f>((E35-C35)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="36" ht="14.4" customHeight="true">
-      <c r="B36" s="46" t="n">
+      <c r="B36" s="296" t="n">
         <v>21.0</v>
       </c>
-      <c r="C36" s="46"/>
-      <c r="E36" s="46"/>
-      <c r="G36" s="46" t="s">
-        <v>83</v>
+      <c r="C36" s="297"/>
+      <c r="E36" s="297"/>
+      <c r="G36" s="295" t="n">
+        <f>((E36-C36)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="37" ht="14.4" customHeight="true">
-      <c r="B37" s="46" t="n">
+      <c r="B37" s="296" t="n">
         <v>22.0</v>
       </c>
-      <c r="C37" s="46"/>
-      <c r="E37" s="46"/>
-      <c r="G37" s="46" t="s">
-        <v>83</v>
+      <c r="C37" s="297"/>
+      <c r="E37" s="297"/>
+      <c r="G37" s="295" t="n">
+        <f>((E37-C37)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="38" ht="14.4" customHeight="true">
-      <c r="B38" s="46" t="n">
+      <c r="B38" s="296" t="n">
         <v>23.0</v>
       </c>
-      <c r="C38" s="46"/>
-      <c r="E38" s="46"/>
-      <c r="G38" s="46" t="s">
-        <v>83</v>
+      <c r="C38" s="297"/>
+      <c r="E38" s="297"/>
+      <c r="G38" s="295" t="n">
+        <f>((E38-C38)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="39" ht="14.4" customHeight="true">
@@ -13847,13 +14071,14 @@
       </c>
     </row>
     <row r="41" ht="14.4" customHeight="true">
-      <c r="B41" s="56" t="n">
+      <c r="B41" s="296" t="n">
         <v>26.0</v>
       </c>
-      <c r="C41" s="56"/>
-      <c r="E41" s="56"/>
-      <c r="G41" s="56" t="s">
-        <v>83</v>
+      <c r="C41" s="297"/>
+      <c r="E41" s="297"/>
+      <c r="G41" s="295" t="n">
+        <f>((E41-C41)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="42" ht="14.4" customHeight="true">
@@ -13867,33 +14092,36 @@
       </c>
     </row>
     <row r="43" ht="14.4" customHeight="true">
-      <c r="B43" s="56" t="n">
+      <c r="B43" s="296" t="n">
         <v>28.0</v>
       </c>
-      <c r="C43" s="56"/>
-      <c r="E43" s="56"/>
-      <c r="G43" s="56" t="s">
-        <v>83</v>
+      <c r="C43" s="297"/>
+      <c r="E43" s="297"/>
+      <c r="G43" s="295" t="n">
+        <f>((E43-C43)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="44" ht="14.4" customHeight="true">
-      <c r="B44" s="56" t="n">
+      <c r="B44" s="296" t="n">
         <v>29.0</v>
       </c>
-      <c r="C44" s="56"/>
-      <c r="E44" s="56"/>
-      <c r="G44" s="56" t="s">
-        <v>83</v>
+      <c r="C44" s="297"/>
+      <c r="E44" s="297"/>
+      <c r="G44" s="295" t="n">
+        <f>((E44-C44)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="45" ht="14.4" customHeight="true">
-      <c r="B45" s="56" t="n">
+      <c r="B45" s="296" t="n">
         <v>30.0</v>
       </c>
-      <c r="C45" s="56"/>
-      <c r="E45" s="56"/>
-      <c r="G45" s="56" t="s">
-        <v>83</v>
+      <c r="C45" s="297"/>
+      <c r="E45" s="297"/>
+      <c r="G45" s="295" t="n">
+        <f>((E45-C45)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="46" ht="14.4" customHeight="true">
@@ -14167,53 +14395,58 @@
       </c>
     </row>
     <row r="17" ht="14.4" customHeight="true">
-      <c r="B17" s="30" t="n">
+      <c r="B17" s="325" t="n">
         <v>2.0</v>
       </c>
-      <c r="C17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="G17" s="30" t="s">
-        <v>83</v>
+      <c r="C17" s="326"/>
+      <c r="E17" s="326"/>
+      <c r="G17" s="324" t="n">
+        <f>((E17-C17)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="18" ht="14.4" customHeight="true">
-      <c r="B18" s="30" t="n">
+      <c r="B18" s="325" t="n">
         <v>3.0</v>
       </c>
-      <c r="C18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="G18" s="30" t="s">
-        <v>83</v>
+      <c r="C18" s="326"/>
+      <c r="E18" s="326"/>
+      <c r="G18" s="324" t="n">
+        <f>((E18-C18)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="19" ht="14.4" customHeight="true">
-      <c r="B19" s="30" t="n">
+      <c r="B19" s="325" t="n">
         <v>4.0</v>
       </c>
-      <c r="C19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="G19" s="30" t="s">
-        <v>83</v>
+      <c r="C19" s="326"/>
+      <c r="E19" s="326"/>
+      <c r="G19" s="324" t="n">
+        <f>((E19-C19)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="20" ht="14.4" customHeight="true">
-      <c r="B20" s="30" t="n">
+      <c r="B20" s="325" t="n">
         <v>5.0</v>
       </c>
-      <c r="C20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="G20" s="30" t="s">
-        <v>83</v>
+      <c r="C20" s="326"/>
+      <c r="E20" s="326"/>
+      <c r="G20" s="324" t="n">
+        <f>((E20-C20)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="21" ht="14.4" customHeight="true">
-      <c r="B21" s="30" t="n">
+      <c r="B21" s="325" t="n">
         <v>6.0</v>
       </c>
-      <c r="C21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="G21" s="30" t="s">
-        <v>83</v>
+      <c r="C21" s="326"/>
+      <c r="E21" s="326"/>
+      <c r="G21" s="324" t="n">
+        <f>((E21-C21)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="22" ht="14.4" customHeight="true">
@@ -14237,53 +14470,58 @@
       </c>
     </row>
     <row r="24" ht="14.4" customHeight="true">
-      <c r="B24" s="36" t="n">
+      <c r="B24" s="325" t="n">
         <v>9.0</v>
       </c>
-      <c r="C24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="G24" s="36" t="s">
-        <v>83</v>
+      <c r="C24" s="326"/>
+      <c r="E24" s="326"/>
+      <c r="G24" s="324" t="n">
+        <f>((E24-C24)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="25" ht="14.4" customHeight="true">
-      <c r="B25" s="36" t="n">
+      <c r="B25" s="325" t="n">
         <v>10.0</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="G25" s="36" t="s">
-        <v>83</v>
+      <c r="C25" s="326"/>
+      <c r="E25" s="326"/>
+      <c r="G25" s="324" t="n">
+        <f>((E25-C25)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="26" ht="14.4" customHeight="true">
-      <c r="B26" s="36" t="n">
+      <c r="B26" s="325" t="n">
         <v>11.0</v>
       </c>
-      <c r="C26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="G26" s="36" t="s">
-        <v>83</v>
+      <c r="C26" s="326"/>
+      <c r="E26" s="326"/>
+      <c r="G26" s="324" t="n">
+        <f>((E26-C26)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="27" ht="14.4" customHeight="true">
-      <c r="B27" s="36" t="n">
+      <c r="B27" s="325" t="n">
         <v>12.0</v>
       </c>
-      <c r="C27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="G27" s="36" t="s">
-        <v>83</v>
+      <c r="C27" s="326"/>
+      <c r="E27" s="326"/>
+      <c r="G27" s="324" t="n">
+        <f>((E27-C27)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="28" ht="14.4" customHeight="true">
-      <c r="B28" s="36" t="n">
+      <c r="B28" s="325" t="n">
         <v>13.0</v>
       </c>
-      <c r="C28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="G28" s="36" t="s">
-        <v>83</v>
+      <c r="C28" s="326"/>
+      <c r="E28" s="326"/>
+      <c r="G28" s="324" t="n">
+        <f>((E28-C28)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="29" ht="14.4" customHeight="true">
@@ -14307,53 +14545,58 @@
       </c>
     </row>
     <row r="31" ht="14.4" customHeight="true">
-      <c r="B31" s="43" t="n">
+      <c r="B31" s="325" t="n">
         <v>16.0</v>
       </c>
-      <c r="C31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="G31" s="43" t="s">
-        <v>83</v>
+      <c r="C31" s="326"/>
+      <c r="E31" s="326"/>
+      <c r="G31" s="324" t="n">
+        <f>((E31-C31)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="32" ht="14.4" customHeight="true">
-      <c r="B32" s="43" t="n">
+      <c r="B32" s="325" t="n">
         <v>17.0</v>
       </c>
-      <c r="C32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="G32" s="43" t="s">
-        <v>83</v>
+      <c r="C32" s="326"/>
+      <c r="E32" s="326"/>
+      <c r="G32" s="324" t="n">
+        <f>((E32-C32)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="33" ht="14.4" customHeight="true">
-      <c r="B33" s="43" t="n">
+      <c r="B33" s="325" t="n">
         <v>18.0</v>
       </c>
-      <c r="C33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="G33" s="43" t="s">
-        <v>83</v>
+      <c r="C33" s="326"/>
+      <c r="E33" s="326"/>
+      <c r="G33" s="324" t="n">
+        <f>((E33-C33)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="34" ht="14.4" customHeight="true">
-      <c r="B34" s="43" t="n">
+      <c r="B34" s="325" t="n">
         <v>19.0</v>
       </c>
-      <c r="C34" s="43"/>
-      <c r="E34" s="43"/>
-      <c r="G34" s="43" t="s">
-        <v>83</v>
+      <c r="C34" s="326"/>
+      <c r="E34" s="326"/>
+      <c r="G34" s="324" t="n">
+        <f>((E34-C34)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="35" ht="14.4" customHeight="true">
-      <c r="B35" s="43" t="n">
+      <c r="B35" s="325" t="n">
         <v>20.0</v>
       </c>
-      <c r="C35" s="43"/>
-      <c r="E35" s="43"/>
-      <c r="G35" s="43" t="s">
-        <v>83</v>
+      <c r="C35" s="326"/>
+      <c r="E35" s="326"/>
+      <c r="G35" s="324" t="n">
+        <f>((E35-C35)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="36" ht="14.4" customHeight="true">
@@ -14377,53 +14620,58 @@
       </c>
     </row>
     <row r="38" ht="14.4" customHeight="true">
-      <c r="B38" s="46" t="n">
+      <c r="B38" s="325" t="n">
         <v>23.0</v>
       </c>
-      <c r="C38" s="46"/>
-      <c r="E38" s="46"/>
-      <c r="G38" s="46" t="s">
-        <v>83</v>
+      <c r="C38" s="326"/>
+      <c r="E38" s="326"/>
+      <c r="G38" s="324" t="n">
+        <f>((E38-C38)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="39" ht="14.4" customHeight="true">
-      <c r="B39" s="46" t="n">
+      <c r="B39" s="325" t="n">
         <v>24.0</v>
       </c>
-      <c r="C39" s="46"/>
-      <c r="E39" s="46"/>
-      <c r="G39" s="46" t="s">
-        <v>83</v>
+      <c r="C39" s="326"/>
+      <c r="E39" s="326"/>
+      <c r="G39" s="324" t="n">
+        <f>((E39-C39)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="40" ht="14.4" customHeight="true">
-      <c r="B40" s="46" t="n">
+      <c r="B40" s="325" t="n">
         <v>25.0</v>
       </c>
-      <c r="C40" s="46"/>
-      <c r="E40" s="46"/>
-      <c r="G40" s="46" t="s">
-        <v>83</v>
+      <c r="C40" s="326"/>
+      <c r="E40" s="326"/>
+      <c r="G40" s="324" t="n">
+        <f>((E40-C40)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="41" ht="14.4" customHeight="true">
-      <c r="B41" s="46" t="n">
+      <c r="B41" s="325" t="n">
         <v>26.0</v>
       </c>
-      <c r="C41" s="46"/>
-      <c r="E41" s="46"/>
-      <c r="G41" s="46" t="s">
-        <v>83</v>
+      <c r="C41" s="326"/>
+      <c r="E41" s="326"/>
+      <c r="G41" s="324" t="n">
+        <f>((E41-C41)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="42" ht="14.4" customHeight="true">
-      <c r="B42" s="46" t="n">
+      <c r="B42" s="325" t="n">
         <v>27.0</v>
       </c>
-      <c r="C42" s="46"/>
-      <c r="E42" s="46"/>
-      <c r="G42" s="46" t="s">
-        <v>83</v>
+      <c r="C42" s="326"/>
+      <c r="E42" s="326"/>
+      <c r="G42" s="324" t="n">
+        <f>((E42-C42)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="43" ht="14.4" customHeight="true">
@@ -14447,23 +14695,25 @@
       </c>
     </row>
     <row r="45" ht="14.4" customHeight="true">
-      <c r="B45" s="56" t="n">
+      <c r="B45" s="325" t="n">
         <v>30.0</v>
       </c>
-      <c r="C45" s="56"/>
-      <c r="E45" s="56"/>
-      <c r="G45" s="56" t="s">
-        <v>83</v>
+      <c r="C45" s="326"/>
+      <c r="E45" s="326"/>
+      <c r="G45" s="324" t="n">
+        <f>((E45-C45)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="46" ht="14.4" customHeight="true">
-      <c r="B46" s="57" t="n">
+      <c r="B46" s="325" t="n">
         <v>31.0</v>
       </c>
-      <c r="C46" s="57"/>
-      <c r="E46" s="57"/>
-      <c r="G46" s="57" t="s">
-        <v>83</v>
+      <c r="C46" s="326"/>
+      <c r="E46" s="326"/>
+      <c r="G46" s="324" t="n">
+        <f>((E46-C46)*24)-1</f>
+        <v>0.0</v>
       </c>
     </row>
     <row r="47" ht="14.4" customHeight="true">

</xml_diff>